<commit_message>
Excel: ADX, Williams %R
</commit_message>
<xml_diff>
--- a/tmp/daily_MSFT.xlsx
+++ b/tmp/daily_MSFT.xlsx
@@ -16,7 +16,7 @@
     <sheet name="ADX" sheetId="2" r:id="rId2"/>
     <sheet name="William %R" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -582,7 +582,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -597,6 +597,9 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -922,7 +925,7 @@
   <dimension ref="A1:K250"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -931,35 +934,35 @@
     <col min="11" max="11" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="5" t="s">
@@ -9517,8 +9520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q250"/>
   <sheetViews>
-    <sheetView topLeftCell="A242" workbookViewId="0">
-      <selection sqref="A1:E250"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9530,53 +9533,53 @@
     <col min="17" max="17" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="6" t="s">
         <v>21</v>
       </c>
       <c r="Q1" s="6" t="s">
@@ -25210,7 +25213,7 @@
   <dimension ref="A1:H250"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25219,26 +25222,26 @@
     <col min="8" max="8" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="6" t="s">
         <v>24</v>
       </c>
       <c r="H1" s="6" t="s">
@@ -25483,15 +25486,15 @@
         <v>173.7</v>
       </c>
       <c r="F15">
-        <f>MAX(C2:C15)-E15</f>
+        <f t="shared" ref="F15:F78" si="0">MAX(C2:C15)-E15</f>
         <v>5.0000000000011369E-2</v>
       </c>
       <c r="G15">
-        <f>MAX(C2:C15)-MIN(D2:D15)</f>
+        <f t="shared" ref="G15:G78" si="1">MAX(C2:C15)-MIN(D2:D15)</f>
         <v>29.310000000000002</v>
       </c>
       <c r="H15" s="5">
-        <f>F15/G15*100</f>
+        <f t="shared" ref="H15:H78" si="2">F15/G15*100</f>
         <v>0.17059024223818275</v>
       </c>
     </row>
@@ -25512,15 +25515,15 @@
         <v>171.88</v>
       </c>
       <c r="F16">
-        <f>MAX(C3:C16)-E16</f>
+        <f t="shared" si="0"/>
         <v>1.8700000000000045</v>
       </c>
       <c r="G16">
-        <f>MAX(C3:C16)-MIN(D3:D16)</f>
+        <f t="shared" si="1"/>
         <v>25.379999999999995</v>
       </c>
       <c r="H16" s="5">
-        <f>F16/G16*100</f>
+        <f t="shared" si="2"/>
         <v>7.3680063041765358</v>
       </c>
     </row>
@@ -25541,15 +25544,15 @@
         <v>177.04</v>
       </c>
       <c r="F17">
-        <f>MAX(C4:C17)-E17</f>
+        <f t="shared" si="0"/>
         <v>0.24000000000000909</v>
       </c>
       <c r="G17">
-        <f>MAX(C4:C17)-MIN(D4:D17)</f>
+        <f t="shared" si="1"/>
         <v>28.080000000000013</v>
       </c>
       <c r="H17" s="5">
-        <f>F17/G17*100</f>
+        <f t="shared" si="2"/>
         <v>0.85470085470088675</v>
       </c>
     </row>
@@ -25570,15 +25573,15 @@
         <v>178.6</v>
       </c>
       <c r="F18">
-        <f>MAX(C5:C18)-E18</f>
+        <f t="shared" si="0"/>
         <v>1.4000000000000057</v>
       </c>
       <c r="G18">
-        <f>MAX(C5:C18)-MIN(D5:D18)</f>
+        <f t="shared" si="1"/>
         <v>29.990000000000009</v>
       </c>
       <c r="H18" s="5">
-        <f>F18/G18*100</f>
+        <f t="shared" si="2"/>
         <v>4.668222740913655</v>
       </c>
     </row>
@@ -25599,15 +25602,15 @@
         <v>175.06</v>
       </c>
       <c r="F19">
-        <f>MAX(C6:C19)-E19</f>
+        <f t="shared" si="0"/>
         <v>4.9399999999999977</v>
       </c>
       <c r="G19">
-        <f>MAX(C6:C19)-MIN(D6:D19)</f>
+        <f t="shared" si="1"/>
         <v>29.639999999999986</v>
       </c>
       <c r="H19" s="5">
-        <f>F19/G19*100</f>
+        <f t="shared" si="2"/>
         <v>16.666666666666664</v>
       </c>
     </row>
@@ -25628,15 +25631,15 @@
         <v>167.82</v>
       </c>
       <c r="F20">
-        <f>MAX(C7:C20)-E20</f>
+        <f t="shared" si="0"/>
         <v>12.180000000000007</v>
       </c>
       <c r="G20">
-        <f>MAX(C7:C20)-MIN(D7:D20)</f>
+        <f t="shared" si="1"/>
         <v>29.639999999999986</v>
       </c>
       <c r="H20" s="5">
-        <f>F20/G20*100</f>
+        <f t="shared" si="2"/>
         <v>41.093117408906927</v>
       </c>
     </row>
@@ -25657,15 +25660,15 @@
         <v>173.52</v>
       </c>
       <c r="F21">
-        <f>MAX(C8:C21)-E21</f>
+        <f t="shared" si="0"/>
         <v>6.4799999999999898</v>
       </c>
       <c r="G21">
-        <f>MAX(C8:C21)-MIN(D8:D21)</f>
+        <f t="shared" si="1"/>
         <v>29.639999999999986</v>
       </c>
       <c r="H21" s="5">
-        <f>F21/G21*100</f>
+        <f t="shared" si="2"/>
         <v>21.862348178137626</v>
       </c>
     </row>
@@ -25686,15 +25689,15 @@
         <v>171.42</v>
       </c>
       <c r="F22">
-        <f>MAX(C9:C22)-E22</f>
+        <f t="shared" si="0"/>
         <v>8.5800000000000125</v>
       </c>
       <c r="G22">
-        <f>MAX(C9:C22)-MIN(D9:D22)</f>
+        <f t="shared" si="1"/>
         <v>27.810000000000002</v>
       </c>
       <c r="H22" s="5">
-        <f>F22/G22*100</f>
+        <f t="shared" si="2"/>
         <v>30.85221143473575</v>
       </c>
     </row>
@@ -25715,15 +25718,15 @@
         <v>174.55</v>
       </c>
       <c r="F23">
-        <f>MAX(C10:C23)-E23</f>
+        <f t="shared" si="0"/>
         <v>5.4499999999999886</v>
       </c>
       <c r="G23">
-        <f>MAX(C10:C23)-MIN(D10:D23)</f>
+        <f t="shared" si="1"/>
         <v>22.419999999999987</v>
       </c>
       <c r="H23" s="5">
-        <f>F23/G23*100</f>
+        <f t="shared" si="2"/>
         <v>24.308652988403175</v>
       </c>
     </row>
@@ -25744,15 +25747,15 @@
         <v>174.05</v>
       </c>
       <c r="F24">
-        <f>MAX(C11:C24)-E24</f>
+        <f t="shared" si="0"/>
         <v>5.9499999999999886</v>
       </c>
       <c r="G24">
-        <f>MAX(C11:C24)-MIN(D11:D24)</f>
+        <f t="shared" si="1"/>
         <v>17.699999999999989</v>
       </c>
       <c r="H24" s="5">
-        <f>F24/G24*100</f>
+        <f t="shared" si="2"/>
         <v>33.615819209039508</v>
       </c>
     </row>
@@ -25773,15 +25776,15 @@
         <v>169.81</v>
       </c>
       <c r="F25">
-        <f>MAX(C12:C25)-E25</f>
+        <f t="shared" si="0"/>
         <v>10.189999999999998</v>
       </c>
       <c r="G25">
-        <f>MAX(C12:C25)-MIN(D12:D25)</f>
+        <f t="shared" si="1"/>
         <v>17.699999999999989</v>
       </c>
       <c r="H25" s="5">
-        <f>F25/G25*100</f>
+        <f t="shared" si="2"/>
         <v>57.570621468926575</v>
       </c>
     </row>
@@ -25802,15 +25805,15 @@
         <v>177.43</v>
       </c>
       <c r="F26">
-        <f>MAX(C13:C26)-E26</f>
+        <f t="shared" si="0"/>
         <v>2.5699999999999932</v>
       </c>
       <c r="G26">
-        <f>MAX(C13:C26)-MIN(D13:D26)</f>
+        <f t="shared" si="1"/>
         <v>17.699999999999989</v>
       </c>
       <c r="H26" s="5">
-        <f>F26/G26*100</f>
+        <f t="shared" si="2"/>
         <v>14.519774011299406</v>
       </c>
     </row>
@@ -25831,15 +25834,15 @@
         <v>179.21</v>
       </c>
       <c r="F27">
-        <f>MAX(C14:C27)-E27</f>
+        <f t="shared" si="0"/>
         <v>1.1899999999999977</v>
       </c>
       <c r="G27">
-        <f>MAX(C14:C27)-MIN(D14:D27)</f>
+        <f t="shared" si="1"/>
         <v>18.099999999999994</v>
       </c>
       <c r="H27" s="5">
-        <f>F27/G27*100</f>
+        <f t="shared" si="2"/>
         <v>6.5745856353591048</v>
       </c>
     </row>
@@ -25860,15 +25863,15 @@
         <v>174.57</v>
       </c>
       <c r="F28">
-        <f>MAX(C15:C28)-E28</f>
+        <f t="shared" si="0"/>
         <v>5.8300000000000125</v>
       </c>
       <c r="G28">
-        <f>MAX(C15:C28)-MIN(D15:D28)</f>
+        <f t="shared" si="1"/>
         <v>14.289999999999992</v>
       </c>
       <c r="H28" s="5">
-        <f>F28/G28*100</f>
+        <f t="shared" si="2"/>
         <v>40.797760671798571</v>
       </c>
     </row>
@@ -25889,15 +25892,15 @@
         <v>178.84</v>
       </c>
       <c r="F29">
-        <f>MAX(C16:C29)-E29</f>
+        <f t="shared" si="0"/>
         <v>1.5600000000000023</v>
       </c>
       <c r="G29">
-        <f>MAX(C16:C29)-MIN(D16:D29)</f>
+        <f t="shared" si="1"/>
         <v>14.289999999999992</v>
       </c>
       <c r="H29" s="5">
-        <f>F29/G29*100</f>
+        <f t="shared" si="2"/>
         <v>10.91672498250527</v>
       </c>
     </row>
@@ -25918,15 +25921,15 @@
         <v>180.76</v>
       </c>
       <c r="F30">
-        <f>MAX(C17:C30)-E30</f>
+        <f t="shared" si="0"/>
         <v>2.8900000000000148</v>
       </c>
       <c r="G30">
-        <f>MAX(C17:C30)-MIN(D17:D30)</f>
+        <f t="shared" si="1"/>
         <v>17.539999999999992</v>
       </c>
       <c r="H30" s="5">
-        <f>F30/G30*100</f>
+        <f t="shared" si="2"/>
         <v>16.476624857468735</v>
       </c>
     </row>
@@ -25947,15 +25950,15 @@
         <v>182.54</v>
       </c>
       <c r="F31">
-        <f>MAX(C18:C31)-E31</f>
+        <f t="shared" si="0"/>
         <v>1.6599999999999966</v>
       </c>
       <c r="G31">
-        <f>MAX(C18:C31)-MIN(D18:D31)</f>
+        <f t="shared" si="1"/>
         <v>18.089999999999975</v>
       </c>
       <c r="H31" s="5">
-        <f>F31/G31*100</f>
+        <f t="shared" si="2"/>
         <v>9.1763405196240964</v>
       </c>
     </row>
@@ -25976,15 +25979,15 @@
         <v>183.6</v>
       </c>
       <c r="F32">
-        <f>MAX(C19:C32)-E32</f>
+        <f t="shared" si="0"/>
         <v>0.95000000000001705</v>
       </c>
       <c r="G32">
-        <f>MAX(C19:C32)-MIN(D19:D32)</f>
+        <f t="shared" si="1"/>
         <v>18.439999999999998</v>
       </c>
       <c r="H32" s="5">
-        <f>F32/G32*100</f>
+        <f t="shared" si="2"/>
         <v>5.1518438177875119</v>
       </c>
     </row>
@@ -26005,15 +26008,15 @@
         <v>184.68</v>
       </c>
       <c r="F33">
-        <f>MAX(C20:C33)-E33</f>
+        <f t="shared" si="0"/>
         <v>0.31999999999999318</v>
       </c>
       <c r="G33">
-        <f>MAX(C20:C33)-MIN(D20:D33)</f>
+        <f t="shared" si="1"/>
         <v>18.889999999999986</v>
       </c>
       <c r="H33" s="5">
-        <f>F33/G33*100</f>
+        <f t="shared" si="2"/>
         <v>1.6940179989412039</v>
       </c>
     </row>
@@ -26034,15 +26037,15 @@
         <v>186.74</v>
       </c>
       <c r="F34">
-        <f>MAX(C21:C34)-E34</f>
+        <f t="shared" si="0"/>
         <v>0.76999999999998181</v>
       </c>
       <c r="G34">
-        <f>MAX(C21:C34)-MIN(D21:D34)</f>
+        <f t="shared" si="1"/>
         <v>18.120000000000005</v>
       </c>
       <c r="H34" s="5">
-        <f>F34/G34*100</f>
+        <f t="shared" si="2"/>
         <v>4.2494481236202075</v>
       </c>
     </row>
@@ -26063,15 +26066,15 @@
         <v>182.51</v>
       </c>
       <c r="F35">
-        <f>MAX(C22:C35)-E35</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G35">
-        <f>MAX(C22:C35)-MIN(D22:D35)</f>
+        <f t="shared" si="1"/>
         <v>18.120000000000005</v>
       </c>
       <c r="H35" s="5">
-        <f>F35/G35*100</f>
+        <f t="shared" si="2"/>
         <v>27.593818984547454</v>
       </c>
     </row>
@@ -26092,15 +26095,15 @@
         <v>179.75</v>
       </c>
       <c r="F36">
-        <f>MAX(C23:C36)-E36</f>
+        <f t="shared" si="0"/>
         <v>7.7599999999999909</v>
       </c>
       <c r="G36">
-        <f>MAX(C23:C36)-MIN(D23:D36)</f>
+        <f t="shared" si="1"/>
         <v>18.120000000000005</v>
       </c>
       <c r="H36" s="5">
-        <f>F36/G36*100</f>
+        <f t="shared" si="2"/>
         <v>42.825607064017603</v>
       </c>
     </row>
@@ -26121,15 +26124,15 @@
         <v>180.53</v>
       </c>
       <c r="F37">
-        <f>MAX(C24:C37)-E37</f>
+        <f t="shared" si="0"/>
         <v>6.9799999999999898</v>
       </c>
       <c r="G37">
-        <f>MAX(C24:C37)-MIN(D24:D37)</f>
+        <f t="shared" si="1"/>
         <v>18.120000000000005</v>
       </c>
       <c r="H37" s="5">
-        <f>F37/G37*100</f>
+        <f t="shared" si="2"/>
         <v>38.520971302428194</v>
       </c>
     </row>
@@ -26150,15 +26153,15 @@
         <v>183.16</v>
       </c>
       <c r="F38">
-        <f>MAX(C25:C38)-E38</f>
+        <f t="shared" si="0"/>
         <v>4.3499999999999943</v>
       </c>
       <c r="G38">
-        <f>MAX(C25:C38)-MIN(D25:D38)</f>
+        <f t="shared" si="1"/>
         <v>18.120000000000005</v>
       </c>
       <c r="H38" s="5">
-        <f>F38/G38*100</f>
+        <f t="shared" si="2"/>
         <v>24.006622516556252</v>
       </c>
     </row>
@@ -26179,15 +26182,15 @@
         <v>184.91</v>
       </c>
       <c r="F39">
-        <f>MAX(C26:C39)-E39</f>
+        <f t="shared" si="0"/>
         <v>2.5999999999999943</v>
       </c>
       <c r="G39">
-        <f>MAX(C26:C39)-MIN(D26:D39)</f>
+        <f t="shared" si="1"/>
         <v>15.629999999999995</v>
       </c>
       <c r="H39" s="5">
-        <f>F39/G39*100</f>
+        <f t="shared" si="2"/>
         <v>16.634676903390883</v>
       </c>
     </row>
@@ -26208,15 +26211,15 @@
         <v>183.63</v>
       </c>
       <c r="F40">
-        <f>MAX(C27:C40)-E40</f>
+        <f t="shared" si="0"/>
         <v>3.8799999999999955</v>
       </c>
       <c r="G40">
-        <f>MAX(C27:C40)-MIN(D27:D40)</f>
+        <f t="shared" si="1"/>
         <v>13.70999999999998</v>
       </c>
       <c r="H40" s="5">
-        <f>F40/G40*100</f>
+        <f t="shared" si="2"/>
         <v>28.300510576221743</v>
       </c>
     </row>
@@ -26237,15 +26240,15 @@
         <v>185.66</v>
       </c>
       <c r="F41">
-        <f>MAX(C28:C41)-E41</f>
+        <f t="shared" si="0"/>
         <v>1.8499999999999943</v>
       </c>
       <c r="G41">
-        <f>MAX(C28:C41)-MIN(D28:D41)</f>
+        <f t="shared" si="1"/>
         <v>13.70999999999998</v>
       </c>
       <c r="H41" s="5">
-        <f>F41/G41*100</f>
+        <f t="shared" si="2"/>
         <v>13.493800145878899</v>
       </c>
     </row>
@@ -26266,15 +26269,15 @@
         <v>183.43</v>
       </c>
       <c r="F42">
-        <f>MAX(C29:C42)-E42</f>
+        <f t="shared" si="0"/>
         <v>4.0799999999999841</v>
       </c>
       <c r="G42">
-        <f>MAX(C29:C42)-MIN(D29:D42)</f>
+        <f t="shared" si="1"/>
         <v>13.70999999999998</v>
       </c>
       <c r="H42" s="5">
-        <f>F42/G42*100</f>
+        <f t="shared" si="2"/>
         <v>29.759299781181547</v>
       </c>
     </row>
@@ -26295,15 +26298,15 @@
         <v>183.51</v>
       </c>
       <c r="F43">
-        <f>MAX(C30:C43)-E43</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G43">
-        <f>MAX(C30:C43)-MIN(D30:D43)</f>
+        <f t="shared" si="1"/>
         <v>11.829999999999984</v>
       </c>
       <c r="H43" s="5">
-        <f>F43/G43*100</f>
+        <f t="shared" si="2"/>
         <v>33.81234150464924</v>
       </c>
     </row>
@@ -26324,15 +26327,15 @@
         <v>181.57</v>
       </c>
       <c r="F44">
-        <f>MAX(C31:C44)-E44</f>
+        <f t="shared" si="0"/>
         <v>5.9399999999999977</v>
       </c>
       <c r="G44">
-        <f>MAX(C31:C44)-MIN(D31:D44)</f>
+        <f t="shared" si="1"/>
         <v>11.829999999999984</v>
       </c>
       <c r="H44" s="5">
-        <f>F44/G44*100</f>
+        <f t="shared" si="2"/>
         <v>50.211327134404101</v>
       </c>
     </row>
@@ -26353,15 +26356,15 @@
         <v>181.81</v>
       </c>
       <c r="F45">
-        <f>MAX(C32:C45)-E45</f>
+        <f t="shared" si="0"/>
         <v>5.6999999999999886</v>
       </c>
       <c r="G45">
-        <f>MAX(C32:C45)-MIN(D32:D45)</f>
+        <f t="shared" si="1"/>
         <v>11.829999999999984</v>
       </c>
       <c r="H45" s="5">
-        <f>F45/G45*100</f>
+        <f t="shared" si="2"/>
         <v>48.182586644125074</v>
       </c>
     </row>
@@ -26382,15 +26385,15 @@
         <v>181.4</v>
       </c>
       <c r="F46">
-        <f>MAX(C33:C46)-E46</f>
+        <f t="shared" si="0"/>
         <v>6.1099999999999852</v>
       </c>
       <c r="G46">
-        <f>MAX(C33:C46)-MIN(D33:D46)</f>
+        <f t="shared" si="1"/>
         <v>11.829999999999984</v>
       </c>
       <c r="H46" s="5">
-        <f>F46/G46*100</f>
+        <f t="shared" si="2"/>
         <v>51.6483516483516</v>
       </c>
     </row>
@@ -26411,15 +26414,15 @@
         <v>183.25</v>
       </c>
       <c r="F47">
-        <f>MAX(C34:C47)-E47</f>
+        <f t="shared" si="0"/>
         <v>4.2599999999999909</v>
       </c>
       <c r="G47">
-        <f>MAX(C34:C47)-MIN(D34:D47)</f>
+        <f t="shared" si="1"/>
         <v>11.829999999999984</v>
       </c>
       <c r="H47" s="5">
-        <f>F47/G47*100</f>
+        <f t="shared" si="2"/>
         <v>36.010143702451366</v>
       </c>
     </row>
@@ -26440,15 +26443,15 @@
         <v>182.83</v>
       </c>
       <c r="F48">
-        <f>MAX(C35:C48)-E48</f>
+        <f t="shared" si="0"/>
         <v>4.2299999999999898</v>
       </c>
       <c r="G48">
-        <f>MAX(C35:C48)-MIN(D35:D48)</f>
+        <f t="shared" si="1"/>
         <v>11.379999999999995</v>
       </c>
       <c r="H48" s="5">
-        <f>F48/G48*100</f>
+        <f t="shared" si="2"/>
         <v>37.170474516695883</v>
       </c>
     </row>
@@ -26469,15 +26472,15 @@
         <v>184.91</v>
       </c>
       <c r="F49">
-        <f>MAX(C36:C49)-E49</f>
+        <f t="shared" si="0"/>
         <v>2.1500000000000057</v>
       </c>
       <c r="G49">
-        <f>MAX(C36:C49)-MIN(D36:D49)</f>
+        <f t="shared" si="1"/>
         <v>11.379999999999995</v>
       </c>
       <c r="H49" s="5">
-        <f>F49/G49*100</f>
+        <f t="shared" si="2"/>
         <v>18.892794376098475</v>
       </c>
     </row>
@@ -26498,15 +26501,15 @@
         <v>185.36</v>
       </c>
       <c r="F50">
-        <f>MAX(C37:C50)-E50</f>
+        <f t="shared" si="0"/>
         <v>1.6999999999999886</v>
       </c>
       <c r="G50">
-        <f>MAX(C37:C50)-MIN(D37:D50)</f>
+        <f t="shared" si="1"/>
         <v>11.379999999999995</v>
       </c>
       <c r="H50" s="5">
-        <f>F50/G50*100</f>
+        <f t="shared" si="2"/>
         <v>14.938488576449819</v>
       </c>
     </row>
@@ -26527,15 +26530,15 @@
         <v>182.92</v>
       </c>
       <c r="F51">
-        <f>MAX(C38:C51)-E51</f>
+        <f t="shared" si="0"/>
         <v>4.1400000000000148</v>
       </c>
       <c r="G51">
-        <f>MAX(C38:C51)-MIN(D38:D51)</f>
+        <f t="shared" si="1"/>
         <v>10.460000000000008</v>
       </c>
       <c r="H51" s="5">
-        <f>F51/G51*100</f>
+        <f t="shared" si="2"/>
         <v>39.579349904397816</v>
       </c>
     </row>
@@ -26556,15 +26559,15 @@
         <v>187.2</v>
       </c>
       <c r="F52">
-        <f>MAX(C39:C52)-E52</f>
+        <f t="shared" si="0"/>
         <v>0.53000000000000114</v>
       </c>
       <c r="G52">
-        <f>MAX(C39:C52)-MIN(D39:D52)</f>
+        <f t="shared" si="1"/>
         <v>11.129999999999995</v>
       </c>
       <c r="H52" s="5">
-        <f>F52/G52*100</f>
+        <f t="shared" si="2"/>
         <v>4.7619047619047743</v>
       </c>
     </row>
@@ -26585,15 +26588,15 @@
         <v>188.36</v>
       </c>
       <c r="F53">
-        <f>MAX(C40:C53)-E53</f>
+        <f t="shared" si="0"/>
         <v>0.18999999999999773</v>
       </c>
       <c r="G53">
-        <f>MAX(C40:C53)-MIN(D40:D53)</f>
+        <f t="shared" si="1"/>
         <v>11.950000000000017</v>
       </c>
       <c r="H53" s="5">
-        <f>F53/G53*100</f>
+        <f t="shared" si="2"/>
         <v>1.5899581589957947</v>
       </c>
     </row>
@@ -26614,15 +26617,15 @@
         <v>189.8</v>
       </c>
       <c r="F54">
-        <f>MAX(C41:C54)-E54</f>
+        <f t="shared" si="0"/>
         <v>0.89999999999997726</v>
       </c>
       <c r="G54">
-        <f>MAX(C41:C54)-MIN(D41:D54)</f>
+        <f t="shared" si="1"/>
         <v>14.099999999999994</v>
       </c>
       <c r="H54" s="5">
-        <f>F54/G54*100</f>
+        <f t="shared" si="2"/>
         <v>6.3829787234040962</v>
       </c>
     </row>
@@ -26643,15 +26646,15 @@
         <v>196.84</v>
       </c>
       <c r="F55">
-        <f>MAX(C42:C55)-E55</f>
+        <f t="shared" si="0"/>
         <v>1.6800000000000068</v>
       </c>
       <c r="G55">
-        <f>MAX(C42:C55)-MIN(D42:D55)</f>
+        <f t="shared" si="1"/>
         <v>21.920000000000016</v>
       </c>
       <c r="H55" s="5">
-        <f>F55/G55*100</f>
+        <f t="shared" si="2"/>
         <v>7.6642335766423608</v>
       </c>
     </row>
@@ -26672,15 +26675,15 @@
         <v>186.27</v>
       </c>
       <c r="F56">
-        <f>MAX(C43:C56)-E56</f>
+        <f t="shared" si="0"/>
         <v>12.25</v>
       </c>
       <c r="G56">
-        <f>MAX(C43:C56)-MIN(D43:D56)</f>
+        <f t="shared" si="1"/>
         <v>21.920000000000016</v>
       </c>
       <c r="H56" s="5">
-        <f>F56/G56*100</f>
+        <f t="shared" si="2"/>
         <v>55.885036496350324</v>
       </c>
     </row>
@@ -26701,15 +26704,15 @@
         <v>187.74</v>
       </c>
       <c r="F57">
-        <f>MAX(C44:C57)-E57</f>
+        <f t="shared" si="0"/>
         <v>10.780000000000001</v>
       </c>
       <c r="G57">
-        <f>MAX(C44:C57)-MIN(D44:D57)</f>
+        <f t="shared" si="1"/>
         <v>21.920000000000016</v>
       </c>
       <c r="H57" s="5">
-        <f>F57/G57*100</f>
+        <f t="shared" si="2"/>
         <v>49.178832116788293</v>
       </c>
     </row>
@@ -26730,15 +26733,15 @@
         <v>188.94</v>
       </c>
       <c r="F58">
-        <f>MAX(C45:C58)-E58</f>
+        <f t="shared" si="0"/>
         <v>9.5800000000000125</v>
       </c>
       <c r="G58">
-        <f>MAX(C45:C58)-MIN(D45:D58)</f>
+        <f t="shared" si="1"/>
         <v>21.920000000000016</v>
       </c>
       <c r="H58" s="5">
-        <f>F58/G58*100</f>
+        <f t="shared" si="2"/>
         <v>43.704379562043819</v>
       </c>
     </row>
@@ -26759,15 +26762,15 @@
         <v>193.57</v>
       </c>
       <c r="F59">
-        <f>MAX(C46:C59)-E59</f>
+        <f t="shared" si="0"/>
         <v>4.9500000000000171</v>
       </c>
       <c r="G59">
-        <f>MAX(C46:C59)-MIN(D46:D59)</f>
+        <f t="shared" si="1"/>
         <v>18.140000000000015</v>
       </c>
       <c r="H59" s="5">
-        <f>F59/G59*100</f>
+        <f t="shared" si="2"/>
         <v>27.287761852260275</v>
       </c>
     </row>
@@ -26788,15 +26791,15 @@
         <v>194.24</v>
       </c>
       <c r="F60">
-        <f>MAX(C47:C60)-E60</f>
+        <f t="shared" si="0"/>
         <v>4.2800000000000011</v>
       </c>
       <c r="G60">
-        <f>MAX(C47:C60)-MIN(D47:D60)</f>
+        <f t="shared" si="1"/>
         <v>18.110000000000014</v>
       </c>
       <c r="H60" s="5">
-        <f>F60/G60*100</f>
+        <f t="shared" si="2"/>
         <v>23.633351739370504</v>
       </c>
     </row>
@@ -26817,15 +26820,15 @@
         <v>196.32</v>
       </c>
       <c r="F61">
-        <f>MAX(C48:C61)-E61</f>
+        <f t="shared" si="0"/>
         <v>2.2000000000000171</v>
       </c>
       <c r="G61">
-        <f>MAX(C48:C61)-MIN(D48:D61)</f>
+        <f t="shared" si="1"/>
         <v>17.170000000000016</v>
       </c>
       <c r="H61" s="5">
-        <f>F61/G61*100</f>
+        <f t="shared" si="2"/>
         <v>12.81304601048349</v>
       </c>
     </row>
@@ -26846,15 +26849,15 @@
         <v>195.15</v>
       </c>
       <c r="F62">
-        <f>MAX(C49:C62)-E62</f>
+        <f t="shared" si="0"/>
         <v>4.1399999999999864</v>
       </c>
       <c r="G62">
-        <f>MAX(C49:C62)-MIN(D49:D62)</f>
+        <f t="shared" si="1"/>
         <v>17.939999999999998</v>
       </c>
       <c r="H62" s="5">
-        <f>F62/G62*100</f>
+        <f t="shared" si="2"/>
         <v>23.076923076923002</v>
       </c>
     </row>
@@ -26875,15 +26878,15 @@
         <v>200.57</v>
       </c>
       <c r="F63">
-        <f>MAX(C50:C63)-E63</f>
+        <f t="shared" si="0"/>
         <v>0.18999999999999773</v>
       </c>
       <c r="G63">
-        <f>MAX(C50:C63)-MIN(D50:D63)</f>
+        <f t="shared" si="1"/>
         <v>18.75</v>
       </c>
       <c r="H63" s="5">
-        <f>F63/G63*100</f>
+        <f t="shared" si="2"/>
         <v>1.0133333333333212</v>
       </c>
     </row>
@@ -26904,15 +26907,15 @@
         <v>201.91</v>
       </c>
       <c r="F64">
-        <f>MAX(C51:C64)-E64</f>
+        <f t="shared" si="0"/>
         <v>2.039999999999992</v>
       </c>
       <c r="G64">
-        <f>MAX(C51:C64)-MIN(D51:D64)</f>
+        <f t="shared" si="1"/>
         <v>21.939999999999998</v>
       </c>
       <c r="H64" s="5">
-        <f>F64/G64*100</f>
+        <f t="shared" si="2"/>
         <v>9.2980856882406204</v>
       </c>
     </row>
@@ -26933,15 +26936,15 @@
         <v>197.84</v>
       </c>
       <c r="F65">
-        <f>MAX(C52:C65)-E65</f>
+        <f t="shared" si="0"/>
         <v>6.1099999999999852</v>
       </c>
       <c r="G65">
-        <f>MAX(C52:C65)-MIN(D52:D65)</f>
+        <f t="shared" si="1"/>
         <v>21.939999999999998</v>
       </c>
       <c r="H65" s="5">
-        <f>F65/G65*100</f>
+        <f t="shared" si="2"/>
         <v>27.848678213308958</v>
       </c>
     </row>
@@ -26962,15 +26965,15 @@
         <v>200.34</v>
       </c>
       <c r="F66">
-        <f>MAX(C53:C66)-E66</f>
+        <f t="shared" si="0"/>
         <v>3.6099999999999852</v>
       </c>
       <c r="G66">
-        <f>MAX(C53:C66)-MIN(D53:D66)</f>
+        <f t="shared" si="1"/>
         <v>19.939999999999998</v>
       </c>
       <c r="H66" s="5">
-        <f>F66/G66*100</f>
+        <f t="shared" si="2"/>
         <v>18.104312938816378</v>
       </c>
     </row>
@@ -26991,15 +26994,15 @@
         <v>196.33</v>
       </c>
       <c r="F67">
-        <f>MAX(C54:C67)-E67</f>
+        <f t="shared" si="0"/>
         <v>7.6199999999999761</v>
       </c>
       <c r="G67">
-        <f>MAX(C54:C67)-MIN(D54:D67)</f>
+        <f t="shared" si="1"/>
         <v>19.939999999999998</v>
       </c>
       <c r="H67" s="5">
-        <f>F67/G67*100</f>
+        <f t="shared" si="2"/>
         <v>38.214643931795273</v>
       </c>
     </row>
@@ -27020,15 +27023,15 @@
         <v>198.44</v>
       </c>
       <c r="F68">
-        <f>MAX(C55:C68)-E68</f>
+        <f t="shared" si="0"/>
         <v>5.5099999999999909</v>
       </c>
       <c r="G68">
-        <f>MAX(C55:C68)-MIN(D55:D68)</f>
+        <f t="shared" si="1"/>
         <v>19.939999999999998</v>
       </c>
       <c r="H68" s="5">
-        <f>F68/G68*100</f>
+        <f t="shared" si="2"/>
         <v>27.632898696088219</v>
       </c>
     </row>
@@ -27049,15 +27052,15 @@
         <v>203.51</v>
       </c>
       <c r="F69">
-        <f>MAX(C56:C69)-E69</f>
+        <f t="shared" si="0"/>
         <v>0.89000000000001478</v>
       </c>
       <c r="G69">
-        <f>MAX(C56:C69)-MIN(D56:D69)</f>
+        <f t="shared" si="1"/>
         <v>20.390000000000015</v>
       </c>
       <c r="H69" s="5">
-        <f>F69/G69*100</f>
+        <f t="shared" si="2"/>
         <v>4.3648847474252781</v>
       </c>
     </row>
@@ -27078,15 +27081,15 @@
         <v>204.7</v>
       </c>
       <c r="F70">
-        <f>MAX(C57:C70)-E70</f>
+        <f t="shared" si="0"/>
         <v>1.6500000000000057</v>
       </c>
       <c r="G70">
-        <f>MAX(C57:C70)-MIN(D57:D70)</f>
+        <f t="shared" si="1"/>
         <v>22.340000000000003</v>
       </c>
       <c r="H70" s="5">
-        <f>F70/G70*100</f>
+        <f t="shared" si="2"/>
         <v>7.385854968666095</v>
       </c>
     </row>
@@ -27107,15 +27110,15 @@
         <v>206.26</v>
       </c>
       <c r="F71">
-        <f>MAX(C58:C71)-E71</f>
+        <f t="shared" si="0"/>
         <v>1.7600000000000193</v>
       </c>
       <c r="G71">
-        <f>MAX(C58:C71)-MIN(D58:D71)</f>
+        <f t="shared" si="1"/>
         <v>24.010000000000019</v>
       </c>
       <c r="H71" s="5">
-        <f>F71/G71*100</f>
+        <f t="shared" si="2"/>
         <v>7.3302790503957427</v>
       </c>
     </row>
@@ -27136,15 +27139,15 @@
         <v>210.7</v>
       </c>
       <c r="F72">
-        <f>MAX(C59:C72)-E72</f>
+        <f t="shared" si="0"/>
         <v>0.43000000000000682</v>
       </c>
       <c r="G72">
-        <f>MAX(C59:C72)-MIN(D59:D72)</f>
+        <f t="shared" si="1"/>
         <v>19.669999999999987</v>
       </c>
       <c r="H72" s="5">
-        <f>F72/G72*100</f>
+        <f t="shared" si="2"/>
         <v>2.1860701576004429</v>
       </c>
     </row>
@@ -27165,15 +27168,15 @@
         <v>208.25</v>
       </c>
       <c r="F73">
-        <f>MAX(C60:C73)-E73</f>
+        <f t="shared" si="0"/>
         <v>6.4199999999999875</v>
       </c>
       <c r="G73">
-        <f>MAX(C60:C73)-MIN(D60:D73)</f>
+        <f t="shared" si="1"/>
         <v>21.119999999999976</v>
       </c>
       <c r="H73" s="5">
-        <f>F73/G73*100</f>
+        <f t="shared" si="2"/>
         <v>30.397727272727249</v>
       </c>
     </row>
@@ -27194,15 +27197,15 @@
         <v>212.83</v>
       </c>
       <c r="F74">
-        <f>MAX(C61:C74)-E74</f>
+        <f t="shared" si="0"/>
         <v>1.839999999999975</v>
       </c>
       <c r="G74">
-        <f>MAX(C61:C74)-MIN(D61:D74)</f>
+        <f t="shared" si="1"/>
         <v>21.119999999999976</v>
       </c>
       <c r="H74" s="5">
-        <f>F74/G74*100</f>
+        <f t="shared" si="2"/>
         <v>8.7121212121211027</v>
       </c>
     </row>
@@ -27223,15 +27226,15 @@
         <v>214.32</v>
       </c>
       <c r="F75">
-        <f>MAX(C62:C75)-E75</f>
+        <f t="shared" si="0"/>
         <v>2.0600000000000023</v>
       </c>
       <c r="G75">
-        <f>MAX(C62:C75)-MIN(D62:D75)</f>
+        <f t="shared" si="1"/>
         <v>22.829999999999984</v>
       </c>
       <c r="H75" s="5">
-        <f>F75/G75*100</f>
+        <f t="shared" si="2"/>
         <v>9.0232150678931387</v>
       </c>
     </row>
@@ -27252,15 +27255,15 @@
         <v>213.67</v>
       </c>
       <c r="F76">
-        <f>MAX(C63:C76)-E76</f>
+        <f t="shared" si="0"/>
         <v>2.710000000000008</v>
       </c>
       <c r="G76">
-        <f>MAX(C63:C76)-MIN(D63:D76)</f>
+        <f t="shared" si="1"/>
         <v>22.829999999999984</v>
       </c>
       <c r="H76" s="5">
-        <f>F76/G76*100</f>
+        <f t="shared" si="2"/>
         <v>11.870346035917695</v>
       </c>
     </row>
@@ -27281,15 +27284,15 @@
         <v>207.07</v>
       </c>
       <c r="F77">
-        <f>MAX(C64:C77)-E77</f>
+        <f t="shared" si="0"/>
         <v>9.3100000000000023</v>
       </c>
       <c r="G77">
-        <f>MAX(C64:C77)-MIN(D64:D77)</f>
+        <f t="shared" si="1"/>
         <v>22.829999999999984</v>
       </c>
       <c r="H77" s="5">
-        <f>F77/G77*100</f>
+        <f t="shared" si="2"/>
         <v>40.779675865089828</v>
       </c>
     </row>
@@ -27310,15 +27313,15 @@
         <v>208.35</v>
       </c>
       <c r="F78">
-        <f>MAX(C65:C78)-E78</f>
+        <f t="shared" si="0"/>
         <v>8.0300000000000011</v>
       </c>
       <c r="G78">
-        <f>MAX(C65:C78)-MIN(D65:D78)</f>
+        <f t="shared" si="1"/>
         <v>22.829999999999984</v>
       </c>
       <c r="H78" s="5">
-        <f>F78/G78*100</f>
+        <f t="shared" si="2"/>
         <v>35.173017958826136</v>
       </c>
     </row>
@@ -27339,15 +27342,15 @@
         <v>208.04</v>
       </c>
       <c r="F79">
-        <f>MAX(C66:C79)-E79</f>
+        <f t="shared" ref="F79:F142" si="3">MAX(C66:C79)-E79</f>
         <v>8.3400000000000034</v>
       </c>
       <c r="G79">
-        <f>MAX(C66:C79)-MIN(D66:D79)</f>
+        <f t="shared" ref="G79:G142" si="4">MAX(C66:C79)-MIN(D66:D79)</f>
         <v>22.829999999999984</v>
       </c>
       <c r="H79" s="5">
-        <f>F79/G79*100</f>
+        <f t="shared" ref="H79:H142" si="5">F79/G79*100</f>
         <v>36.530880420499386</v>
       </c>
     </row>
@@ -27368,15 +27371,15 @@
         <v>203.92</v>
       </c>
       <c r="F80">
-        <f>MAX(C67:C80)-E80</f>
+        <f t="shared" si="3"/>
         <v>12.460000000000008</v>
       </c>
       <c r="G80">
-        <f>MAX(C67:C80)-MIN(D67:D80)</f>
+        <f t="shared" si="4"/>
         <v>22.829999999999984</v>
       </c>
       <c r="H80" s="5">
-        <f>F80/G80*100</f>
+        <f t="shared" si="5"/>
         <v>54.57731055628566</v>
       </c>
     </row>
@@ -27397,15 +27400,15 @@
         <v>202.88</v>
       </c>
       <c r="F81">
-        <f>MAX(C68:C81)-E81</f>
+        <f t="shared" si="3"/>
         <v>13.5</v>
       </c>
       <c r="G81">
-        <f>MAX(C68:C81)-MIN(D68:D81)</f>
+        <f t="shared" si="4"/>
         <v>22.829999999999984</v>
       </c>
       <c r="H81" s="5">
-        <f>F81/G81*100</f>
+        <f t="shared" si="5"/>
         <v>59.132720105124882</v>
       </c>
     </row>
@@ -27426,15 +27429,15 @@
         <v>211.6</v>
       </c>
       <c r="F82">
-        <f>MAX(C69:C82)-E82</f>
+        <f t="shared" si="3"/>
         <v>4.7800000000000011</v>
       </c>
       <c r="G82">
-        <f>MAX(C69:C82)-MIN(D69:D82)</f>
+        <f t="shared" si="4"/>
         <v>18.639999999999986</v>
       </c>
       <c r="H82" s="5">
-        <f>F82/G82*100</f>
+        <f t="shared" si="5"/>
         <v>25.643776824034358</v>
       </c>
     </row>
@@ -27455,15 +27458,15 @@
         <v>208.75</v>
       </c>
       <c r="F83">
-        <f>MAX(C70:C83)-E83</f>
+        <f t="shared" si="3"/>
         <v>7.6299999999999955</v>
       </c>
       <c r="G83">
-        <f>MAX(C70:C83)-MIN(D70:D83)</f>
+        <f t="shared" si="4"/>
         <v>14.990000000000009</v>
       </c>
       <c r="H83" s="5">
-        <f>F83/G83*100</f>
+        <f t="shared" si="5"/>
         <v>50.900600400266782</v>
       </c>
     </row>
@@ -27484,15 +27487,15 @@
         <v>211.75</v>
       </c>
       <c r="F84">
-        <f>MAX(C71:C84)-E84</f>
+        <f t="shared" si="3"/>
         <v>4.6299999999999955</v>
       </c>
       <c r="G84">
-        <f>MAX(C71:C84)-MIN(D71:D84)</f>
+        <f t="shared" si="4"/>
         <v>14.990000000000009</v>
       </c>
       <c r="H84" s="5">
-        <f>F84/G84*100</f>
+        <f t="shared" si="5"/>
         <v>30.887258172114695</v>
       </c>
     </row>
@@ -27513,15 +27516,15 @@
         <v>202.54</v>
       </c>
       <c r="F85">
-        <f>MAX(C72:C85)-E85</f>
+        <f t="shared" si="3"/>
         <v>13.840000000000003</v>
       </c>
       <c r="G85">
-        <f>MAX(C72:C85)-MIN(D72:D85)</f>
+        <f t="shared" si="4"/>
         <v>14.990000000000009</v>
       </c>
       <c r="H85" s="5">
-        <f>F85/G85*100</f>
+        <f t="shared" si="5"/>
         <v>92.328218812541664</v>
       </c>
     </row>
@@ -27542,15 +27545,15 @@
         <v>201.3</v>
       </c>
       <c r="F86">
-        <f>MAX(C73:C86)-E86</f>
+        <f t="shared" si="3"/>
         <v>15.079999999999984</v>
       </c>
       <c r="G86">
-        <f>MAX(C73:C86)-MIN(D73:D86)</f>
+        <f t="shared" si="4"/>
         <v>18.870000000000005</v>
       </c>
       <c r="H86" s="5">
-        <f>F86/G86*100</f>
+        <f t="shared" si="5"/>
         <v>79.915209326973923</v>
       </c>
     </row>
@@ -27571,15 +27574,15 @@
         <v>203.85</v>
       </c>
       <c r="F87">
-        <f>MAX(C74:C87)-E87</f>
+        <f t="shared" si="3"/>
         <v>12.530000000000001</v>
       </c>
       <c r="G87">
-        <f>MAX(C74:C87)-MIN(D74:D87)</f>
+        <f t="shared" si="4"/>
         <v>18.870000000000005</v>
       </c>
       <c r="H87" s="5">
-        <f>F87/G87*100</f>
+        <f t="shared" si="5"/>
         <v>66.401695813460506</v>
       </c>
     </row>
@@ -27600,15 +27603,15 @@
         <v>202.02</v>
       </c>
       <c r="F88">
-        <f>MAX(C75:C88)-E88</f>
+        <f t="shared" si="3"/>
         <v>14.359999999999985</v>
       </c>
       <c r="G88">
-        <f>MAX(C75:C88)-MIN(D75:D88)</f>
+        <f t="shared" si="4"/>
         <v>18.870000000000005</v>
       </c>
       <c r="H88" s="5">
-        <f>F88/G88*100</f>
+        <f t="shared" si="5"/>
         <v>76.099629040805411</v>
       </c>
     </row>
@@ -27629,15 +27632,15 @@
         <v>204.06</v>
       </c>
       <c r="F89">
-        <f>MAX(C76:C89)-E89</f>
+        <f t="shared" si="3"/>
         <v>11.740000000000009</v>
       </c>
       <c r="G89">
-        <f>MAX(C76:C89)-MIN(D76:D89)</f>
+        <f t="shared" si="4"/>
         <v>18.29000000000002</v>
       </c>
       <c r="H89" s="5">
-        <f>F89/G89*100</f>
+        <f t="shared" si="5"/>
         <v>64.188080918534695</v>
       </c>
     </row>
@@ -27658,15 +27661,15 @@
         <v>203.9</v>
       </c>
       <c r="F90">
-        <f>MAX(C77:C90)-E90</f>
+        <f t="shared" si="3"/>
         <v>11.900000000000006</v>
       </c>
       <c r="G90">
-        <f>MAX(C77:C90)-MIN(D77:D90)</f>
+        <f t="shared" si="4"/>
         <v>18.29000000000002</v>
       </c>
       <c r="H90" s="5">
-        <f>F90/G90*100</f>
+        <f t="shared" si="5"/>
         <v>65.062875888463594</v>
       </c>
     </row>
@@ -27687,15 +27690,15 @@
         <v>205.01</v>
       </c>
       <c r="F91">
-        <f>MAX(C78:C91)-E91</f>
+        <f t="shared" si="3"/>
         <v>8.9300000000000068</v>
       </c>
       <c r="G91">
-        <f>MAX(C78:C91)-MIN(D78:D91)</f>
+        <f t="shared" si="4"/>
         <v>16.430000000000007</v>
       </c>
       <c r="H91" s="5">
-        <f>F91/G91*100</f>
+        <f t="shared" si="5"/>
         <v>54.351795496043842</v>
       </c>
     </row>
@@ -27716,15 +27719,15 @@
         <v>216.54</v>
       </c>
       <c r="F92">
-        <f>MAX(C79:C92)-E92</f>
+        <f t="shared" si="3"/>
         <v>1.0999999999999943</v>
       </c>
       <c r="G92">
-        <f>MAX(C79:C92)-MIN(D79:D92)</f>
+        <f t="shared" si="4"/>
         <v>20.129999999999995</v>
       </c>
       <c r="H92" s="5">
-        <f>F92/G92*100</f>
+        <f t="shared" si="5"/>
         <v>5.4644808743169122</v>
       </c>
     </row>
@@ -27745,15 +27748,15 @@
         <v>213.29</v>
       </c>
       <c r="F93">
-        <f>MAX(C80:C93)-E93</f>
+        <f t="shared" si="3"/>
         <v>4.3499999999999943</v>
       </c>
       <c r="G93">
-        <f>MAX(C80:C93)-MIN(D80:D93)</f>
+        <f t="shared" si="4"/>
         <v>20.129999999999995</v>
       </c>
       <c r="H93" s="5">
-        <f>F93/G93*100</f>
+        <f t="shared" si="5"/>
         <v>21.609538002980603</v>
       </c>
     </row>
@@ -27774,15 +27777,15 @@
         <v>212.94</v>
       </c>
       <c r="F94">
-        <f>MAX(C81:C94)-E94</f>
+        <f t="shared" si="3"/>
         <v>4.6999999999999886</v>
       </c>
       <c r="G94">
-        <f>MAX(C81:C94)-MIN(D81:D94)</f>
+        <f t="shared" si="4"/>
         <v>20.129999999999995</v>
       </c>
       <c r="H94" s="5">
-        <f>F94/G94*100</f>
+        <f t="shared" si="5"/>
         <v>23.34823646299051</v>
       </c>
     </row>
@@ -27803,15 +27806,15 @@
         <v>216.35</v>
       </c>
       <c r="F95">
-        <f>MAX(C82:C95)-E95</f>
+        <f t="shared" si="3"/>
         <v>1.289999999999992</v>
       </c>
       <c r="G95">
-        <f>MAX(C82:C95)-MIN(D82:D95)</f>
+        <f t="shared" si="4"/>
         <v>20.129999999999995</v>
       </c>
       <c r="H95" s="5">
-        <f>F95/G95*100</f>
+        <f t="shared" si="5"/>
         <v>6.4083457526080094</v>
       </c>
     </row>
@@ -27832,15 +27835,15 @@
         <v>212.48</v>
       </c>
       <c r="F96">
-        <f>MAX(C83:C96)-E96</f>
+        <f t="shared" si="3"/>
         <v>5.1599999999999966</v>
       </c>
       <c r="G96">
-        <f>MAX(C83:C96)-MIN(D83:D96)</f>
+        <f t="shared" si="4"/>
         <v>20.129999999999995</v>
       </c>
       <c r="H96" s="5">
-        <f>F96/G96*100</f>
+        <f t="shared" si="5"/>
         <v>25.63338301043218</v>
       </c>
     </row>
@@ -27861,15 +27864,15 @@
         <v>208.25</v>
       </c>
       <c r="F97">
-        <f>MAX(C84:C97)-E97</f>
+        <f t="shared" si="3"/>
         <v>9.3899999999999864</v>
       </c>
       <c r="G97">
-        <f>MAX(C84:C97)-MIN(D84:D97)</f>
+        <f t="shared" si="4"/>
         <v>20.129999999999995</v>
       </c>
       <c r="H97" s="5">
-        <f>F97/G97*100</f>
+        <f t="shared" si="5"/>
         <v>46.64679582712364</v>
       </c>
     </row>
@@ -27890,15 +27893,15 @@
         <v>203.38</v>
       </c>
       <c r="F98">
-        <f>MAX(C85:C98)-E98</f>
+        <f t="shared" si="3"/>
         <v>14.259999999999991</v>
       </c>
       <c r="G98">
-        <f>MAX(C85:C98)-MIN(D85:D98)</f>
+        <f t="shared" si="4"/>
         <v>20.129999999999995</v>
       </c>
       <c r="H98" s="5">
-        <f>F98/G98*100</f>
+        <f t="shared" si="5"/>
         <v>70.839542970690488</v>
       </c>
     </row>
@@ -27919,15 +27922,15 @@
         <v>209.19</v>
       </c>
       <c r="F99">
-        <f>MAX(C86:C99)-E99</f>
+        <f t="shared" si="3"/>
         <v>8.4499999999999886</v>
       </c>
       <c r="G99">
-        <f>MAX(C86:C99)-MIN(D86:D99)</f>
+        <f t="shared" si="4"/>
         <v>20.129999999999995</v>
       </c>
       <c r="H99" s="5">
-        <f>F99/G99*100</f>
+        <f t="shared" si="5"/>
         <v>41.97714853452554</v>
       </c>
     </row>
@@ -27948,15 +27951,15 @@
         <v>208.7</v>
       </c>
       <c r="F100">
-        <f>MAX(C87:C100)-E100</f>
+        <f t="shared" si="3"/>
         <v>8.9399999999999977</v>
       </c>
       <c r="G100">
-        <f>MAX(C87:C100)-MIN(D87:D100)</f>
+        <f t="shared" si="4"/>
         <v>18.629999999999995</v>
       </c>
       <c r="H100" s="5">
-        <f>F100/G100*100</f>
+        <f t="shared" si="5"/>
         <v>47.987117552334944</v>
       </c>
     </row>
@@ -27977,15 +27980,15 @@
         <v>208.9</v>
       </c>
       <c r="F101">
-        <f>MAX(C88:C101)-E101</f>
+        <f t="shared" si="3"/>
         <v>8.7399999999999807</v>
       </c>
       <c r="G101">
-        <f>MAX(C88:C101)-MIN(D88:D101)</f>
+        <f t="shared" si="4"/>
         <v>18.629999999999995</v>
       </c>
       <c r="H101" s="5">
-        <f>F101/G101*100</f>
+        <f t="shared" si="5"/>
         <v>46.91358024691349</v>
       </c>
     </row>
@@ -28006,15 +28009,15 @@
         <v>210.28</v>
       </c>
       <c r="F102">
-        <f>MAX(C89:C102)-E102</f>
+        <f t="shared" si="3"/>
         <v>7.3599999999999852</v>
       </c>
       <c r="G102">
-        <f>MAX(C89:C102)-MIN(D89:D102)</f>
+        <f t="shared" si="4"/>
         <v>18.629999999999995</v>
       </c>
       <c r="H102" s="5">
-        <f>F102/G102*100</f>
+        <f t="shared" si="5"/>
         <v>39.506172839506107</v>
       </c>
     </row>
@@ -28035,15 +28038,15 @@
         <v>211.49</v>
       </c>
       <c r="F103">
-        <f>MAX(C90:C103)-E103</f>
+        <f t="shared" si="3"/>
         <v>6.1499999999999773</v>
       </c>
       <c r="G103">
-        <f>MAX(C90:C103)-MIN(D90:D103)</f>
+        <f t="shared" si="4"/>
         <v>18.629999999999995</v>
       </c>
       <c r="H103" s="5">
-        <f>F103/G103*100</f>
+        <f t="shared" si="5"/>
         <v>33.011272141706812</v>
       </c>
     </row>
@@ -28064,15 +28067,15 @@
         <v>209.7</v>
       </c>
       <c r="F104">
-        <f>MAX(C91:C104)-E104</f>
+        <f t="shared" si="3"/>
         <v>7.9399999999999977</v>
       </c>
       <c r="G104">
-        <f>MAX(C91:C104)-MIN(D91:D104)</f>
+        <f t="shared" si="4"/>
         <v>18.629999999999995</v>
       </c>
       <c r="H104" s="5">
-        <f>F104/G104*100</f>
+        <f t="shared" si="5"/>
         <v>42.619431025228124</v>
       </c>
     </row>
@@ -28093,15 +28096,15 @@
         <v>214.58</v>
       </c>
       <c r="F105">
-        <f>MAX(C92:C105)-E105</f>
+        <f t="shared" si="3"/>
         <v>3.0599999999999739</v>
       </c>
       <c r="G105">
-        <f>MAX(C92:C105)-MIN(D92:D105)</f>
+        <f t="shared" si="4"/>
         <v>14.5</v>
       </c>
       <c r="H105" s="5">
-        <f>F105/G105*100</f>
+        <f t="shared" si="5"/>
         <v>21.10344827586189</v>
       </c>
     </row>
@@ -28122,15 +28125,15 @@
         <v>213.02</v>
       </c>
       <c r="F106">
-        <f>MAX(C93:C106)-E106</f>
+        <f t="shared" si="3"/>
         <v>3.3504999999999825</v>
       </c>
       <c r="G106">
-        <f>MAX(C93:C106)-MIN(D93:D106)</f>
+        <f t="shared" si="4"/>
         <v>13.230500000000006</v>
       </c>
       <c r="H106" s="5">
-        <f>F106/G106*100</f>
+        <f t="shared" si="5"/>
         <v>25.324061826839355</v>
       </c>
     </row>
@@ -28151,15 +28154,15 @@
         <v>213.69</v>
       </c>
       <c r="F107">
-        <f>MAX(C94:C107)-E107</f>
+        <f t="shared" si="3"/>
         <v>2.680499999999995</v>
       </c>
       <c r="G107">
-        <f>MAX(C94:C107)-MIN(D94:D107)</f>
+        <f t="shared" si="4"/>
         <v>13.230500000000006</v>
       </c>
       <c r="H107" s="5">
-        <f>F107/G107*100</f>
+        <f t="shared" si="5"/>
         <v>20.260005290805289</v>
       </c>
     </row>
@@ -28180,15 +28183,15 @@
         <v>216.47</v>
       </c>
       <c r="F108">
-        <f>MAX(C95:C108)-E108</f>
+        <f t="shared" si="3"/>
         <v>0.14000000000001478</v>
       </c>
       <c r="G108">
-        <f>MAX(C95:C108)-MIN(D95:D108)</f>
+        <f t="shared" si="4"/>
         <v>13.470000000000027</v>
       </c>
       <c r="H108" s="5">
-        <f>F108/G108*100</f>
+        <f t="shared" si="5"/>
         <v>1.0393466963623941</v>
       </c>
     </row>
@@ -28209,15 +28212,15 @@
         <v>221.15</v>
       </c>
       <c r="F109">
-        <f>MAX(C96:C109)-E109</f>
+        <f t="shared" si="3"/>
         <v>0.93999999999999773</v>
       </c>
       <c r="G109">
-        <f>MAX(C96:C109)-MIN(D96:D109)</f>
+        <f t="shared" si="4"/>
         <v>18.950000000000017</v>
       </c>
       <c r="H109" s="5">
-        <f>F109/G109*100</f>
+        <f t="shared" si="5"/>
         <v>4.9604221635883743</v>
       </c>
     </row>
@@ -28238,15 +28241,15 @@
         <v>226.58</v>
       </c>
       <c r="F110">
-        <f>MAX(C97:C110)-E110</f>
+        <f t="shared" si="3"/>
         <v>4.5699999999999932</v>
       </c>
       <c r="G110">
-        <f>MAX(C97:C110)-MIN(D97:D110)</f>
+        <f t="shared" si="4"/>
         <v>28.010000000000019</v>
       </c>
       <c r="H110" s="5">
-        <f>F110/G110*100</f>
+        <f t="shared" si="5"/>
         <v>16.315601570867511</v>
       </c>
     </row>
@@ -28267,15 +28270,15 @@
         <v>228.91</v>
       </c>
       <c r="F111">
-        <f>MAX(C98:C111)-E111</f>
+        <f t="shared" si="3"/>
         <v>2.2400000000000091</v>
       </c>
       <c r="G111">
-        <f>MAX(C98:C111)-MIN(D98:D111)</f>
+        <f t="shared" si="4"/>
         <v>28.010000000000019</v>
       </c>
       <c r="H111" s="5">
-        <f>F111/G111*100</f>
+        <f t="shared" si="5"/>
         <v>7.9971438771867467</v>
       </c>
     </row>
@@ -28296,15 +28299,15 @@
         <v>225.53</v>
       </c>
       <c r="F112">
-        <f>MAX(C99:C112)-E112</f>
+        <f t="shared" si="3"/>
         <v>5.6200000000000045</v>
       </c>
       <c r="G112">
-        <f>MAX(C99:C112)-MIN(D99:D112)</f>
+        <f t="shared" si="4"/>
         <v>26.400000000000006</v>
       </c>
       <c r="H112" s="5">
-        <f>F112/G112*100</f>
+        <f t="shared" si="5"/>
         <v>21.2878787878788</v>
       </c>
     </row>
@@ -28325,15 +28328,15 @@
         <v>227.27</v>
       </c>
       <c r="F113">
-        <f>MAX(C100:C113)-E113</f>
+        <f t="shared" si="3"/>
         <v>3.8799999999999955</v>
       </c>
       <c r="G113">
-        <f>MAX(C100:C113)-MIN(D100:D113)</f>
+        <f t="shared" si="4"/>
         <v>23.640000000000015</v>
       </c>
       <c r="H113" s="5">
-        <f>F113/G113*100</f>
+        <f t="shared" si="5"/>
         <v>16.412859560067652</v>
       </c>
     </row>
@@ -28354,15 +28357,15 @@
         <v>231.65</v>
       </c>
       <c r="F114">
-        <f>MAX(C101:C114)-E114</f>
+        <f t="shared" si="3"/>
         <v>1.210000000000008</v>
       </c>
       <c r="G114">
-        <f>MAX(C101:C114)-MIN(D101:D114)</f>
+        <f t="shared" si="4"/>
         <v>25.350000000000023</v>
       </c>
       <c r="H114" s="5">
-        <f>F114/G114*100</f>
+        <f t="shared" si="5"/>
         <v>4.7731755424063387</v>
       </c>
     </row>
@@ -28383,15 +28386,15 @@
         <v>217.3</v>
       </c>
       <c r="F115">
-        <f>MAX(C102:C115)-E115</f>
+        <f t="shared" si="3"/>
         <v>15.560000000000002</v>
       </c>
       <c r="G115">
-        <f>MAX(C102:C115)-MIN(D102:D115)</f>
+        <f t="shared" si="4"/>
         <v>23.950000000000017</v>
       </c>
       <c r="H115" s="5">
-        <f>F115/G115*100</f>
+        <f t="shared" si="5"/>
         <v>64.968684759916457</v>
       </c>
     </row>
@@ -28412,15 +28415,15 @@
         <v>214.25</v>
       </c>
       <c r="F116">
-        <f>MAX(C103:C116)-E116</f>
+        <f t="shared" si="3"/>
         <v>18.610000000000014</v>
       </c>
       <c r="G116">
-        <f>MAX(C103:C116)-MIN(D103:D116)</f>
+        <f t="shared" si="4"/>
         <v>27.670000000000016</v>
       </c>
       <c r="H116" s="5">
-        <f>F116/G116*100</f>
+        <f t="shared" si="5"/>
         <v>67.256956993133372</v>
       </c>
     </row>
@@ -28441,15 +28444,15 @@
         <v>202.66</v>
       </c>
       <c r="F117">
-        <f>MAX(C104:C117)-E117</f>
+        <f t="shared" si="3"/>
         <v>30.200000000000017</v>
       </c>
       <c r="G117">
-        <f>MAX(C104:C117)-MIN(D104:D117)</f>
+        <f t="shared" si="4"/>
         <v>30.660000000000025</v>
       </c>
       <c r="H117" s="5">
-        <f>F117/G117*100</f>
+        <f t="shared" si="5"/>
         <v>98.499673842139572</v>
       </c>
     </row>
@@ -28470,15 +28473,15 @@
         <v>211.29</v>
       </c>
       <c r="F118">
-        <f>MAX(C105:C118)-E118</f>
+        <f t="shared" si="3"/>
         <v>21.570000000000022</v>
       </c>
       <c r="G118">
-        <f>MAX(C105:C118)-MIN(D105:D118)</f>
+        <f t="shared" si="4"/>
         <v>30.660000000000025</v>
       </c>
       <c r="H118" s="5">
-        <f>F118/G118*100</f>
+        <f t="shared" si="5"/>
         <v>70.352250489236795</v>
       </c>
     </row>
@@ -28499,15 +28502,15 @@
         <v>205.37</v>
       </c>
       <c r="F119">
-        <f>MAX(C106:C119)-E119</f>
+        <f t="shared" si="3"/>
         <v>27.490000000000009</v>
       </c>
       <c r="G119">
-        <f>MAX(C106:C119)-MIN(D106:D119)</f>
+        <f t="shared" si="4"/>
         <v>30.660000000000025</v>
       </c>
       <c r="H119" s="5">
-        <f>F119/G119*100</f>
+        <f t="shared" si="5"/>
         <v>89.660795825179335</v>
       </c>
     </row>
@@ -28528,15 +28531,15 @@
         <v>204.03</v>
       </c>
       <c r="F120">
-        <f>MAX(C107:C120)-E120</f>
+        <f t="shared" si="3"/>
         <v>28.830000000000013</v>
       </c>
       <c r="G120">
-        <f>MAX(C107:C120)-MIN(D107:D120)</f>
+        <f t="shared" si="4"/>
         <v>31.620000000000005</v>
       </c>
       <c r="H120" s="5">
-        <f>F120/G120*100</f>
+        <f t="shared" si="5"/>
         <v>91.176470588235333</v>
       </c>
     </row>
@@ -28557,15 +28560,15 @@
         <v>205.41</v>
       </c>
       <c r="F121">
-        <f>MAX(C108:C121)-E121</f>
+        <f t="shared" si="3"/>
         <v>27.450000000000017</v>
       </c>
       <c r="G121">
-        <f>MAX(C108:C121)-MIN(D108:D121)</f>
+        <f t="shared" si="4"/>
         <v>31.620000000000005</v>
       </c>
       <c r="H121" s="5">
-        <f>F121/G121*100</f>
+        <f t="shared" si="5"/>
         <v>86.812144212523762</v>
       </c>
     </row>
@@ -28586,15 +28589,15 @@
         <v>208.78</v>
       </c>
       <c r="F122">
-        <f>MAX(C109:C122)-E122</f>
+        <f t="shared" si="3"/>
         <v>24.080000000000013</v>
       </c>
       <c r="G122">
-        <f>MAX(C109:C122)-MIN(D109:D122)</f>
+        <f t="shared" si="4"/>
         <v>31.620000000000005</v>
       </c>
       <c r="H122" s="5">
-        <f>F122/G122*100</f>
+        <f t="shared" si="5"/>
         <v>76.154332700822295</v>
       </c>
     </row>
@@ -28615,15 +28618,15 @@
         <v>205.05</v>
       </c>
       <c r="F123">
-        <f>MAX(C110:C123)-E123</f>
+        <f t="shared" si="3"/>
         <v>27.810000000000002</v>
       </c>
       <c r="G123">
-        <f>MAX(C110:C123)-MIN(D110:D123)</f>
+        <f t="shared" si="4"/>
         <v>31.620000000000005</v>
       </c>
       <c r="H123" s="5">
-        <f>F123/G123*100</f>
+        <f t="shared" si="5"/>
         <v>87.950664136622379</v>
       </c>
     </row>
@@ -28644,15 +28647,15 @@
         <v>202.91</v>
       </c>
       <c r="F124">
-        <f>MAX(C111:C124)-E124</f>
+        <f t="shared" si="3"/>
         <v>29.950000000000017</v>
       </c>
       <c r="G124">
-        <f>MAX(C111:C124)-MIN(D111:D124)</f>
+        <f t="shared" si="4"/>
         <v>32.900000000000006</v>
       </c>
       <c r="H124" s="5">
-        <f>F124/G124*100</f>
+        <f t="shared" si="5"/>
         <v>91.033434650455959</v>
       </c>
     </row>
@@ -28673,15 +28676,15 @@
         <v>200.39</v>
       </c>
       <c r="F125">
-        <f>MAX(C112:C125)-E125</f>
+        <f t="shared" si="3"/>
         <v>32.470000000000027</v>
       </c>
       <c r="G125">
-        <f>MAX(C112:C125)-MIN(D112:D125)</f>
+        <f t="shared" si="4"/>
         <v>36.610000000000014</v>
       </c>
       <c r="H125" s="5">
-        <f>F125/G125*100</f>
+        <f t="shared" si="5"/>
         <v>88.691614313029262</v>
       </c>
     </row>
@@ -28702,15 +28705,15 @@
         <v>202.54</v>
       </c>
       <c r="F126">
-        <f>MAX(C113:C126)-E126</f>
+        <f t="shared" si="3"/>
         <v>30.320000000000022</v>
       </c>
       <c r="G126">
-        <f>MAX(C113:C126)-MIN(D113:D126)</f>
+        <f t="shared" si="4"/>
         <v>36.610000000000014</v>
       </c>
       <c r="H126" s="5">
-        <f>F126/G126*100</f>
+        <f t="shared" si="5"/>
         <v>82.818901939360856</v>
       </c>
     </row>
@@ -28731,15 +28734,15 @@
         <v>207.42</v>
       </c>
       <c r="F127">
-        <f>MAX(C114:C127)-E127</f>
+        <f t="shared" si="3"/>
         <v>25.440000000000026</v>
       </c>
       <c r="G127">
-        <f>MAX(C114:C127)-MIN(D114:D127)</f>
+        <f t="shared" si="4"/>
         <v>36.610000000000014</v>
       </c>
       <c r="H127" s="5">
-        <f>F127/G127*100</f>
+        <f t="shared" si="5"/>
         <v>69.489210598197261</v>
       </c>
     </row>
@@ -28760,15 +28763,15 @@
         <v>200.59</v>
       </c>
       <c r="F128">
-        <f>MAX(C115:C128)-E128</f>
+        <f t="shared" si="3"/>
         <v>28.72</v>
       </c>
       <c r="G128">
-        <f>MAX(C115:C128)-MIN(D115:D128)</f>
+        <f t="shared" si="4"/>
         <v>33.06</v>
       </c>
       <c r="H128" s="5">
-        <f>F128/G128*100</f>
+        <f t="shared" si="5"/>
         <v>86.872353297035687</v>
       </c>
     </row>
@@ -28789,15 +28792,15 @@
         <v>203.19</v>
       </c>
       <c r="F129">
-        <f>MAX(C116:C129)-E129</f>
+        <f t="shared" si="3"/>
         <v>15.169900000000013</v>
       </c>
       <c r="G129">
-        <f>MAX(C116:C129)-MIN(D116:D129)</f>
+        <f t="shared" si="4"/>
         <v>22.10990000000001</v>
       </c>
       <c r="H129" s="5">
-        <f>F129/G129*100</f>
+        <f t="shared" si="5"/>
         <v>68.611346048602684</v>
       </c>
     </row>
@@ -28818,15 +28821,15 @@
         <v>207.82</v>
       </c>
       <c r="F130">
-        <f>MAX(C117:C130)-E130</f>
+        <f t="shared" si="3"/>
         <v>7.0199000000000069</v>
       </c>
       <c r="G130">
-        <f>MAX(C117:C130)-MIN(D117:D130)</f>
+        <f t="shared" si="4"/>
         <v>18.5899</v>
       </c>
       <c r="H130" s="5">
-        <f>F130/G130*100</f>
+        <f t="shared" si="5"/>
         <v>37.761902968816436</v>
       </c>
     </row>
@@ -28847,15 +28850,15 @@
         <v>209.44</v>
       </c>
       <c r="F131">
-        <f>MAX(C118:C131)-E131</f>
+        <f t="shared" si="3"/>
         <v>5.3999000000000024</v>
       </c>
       <c r="G131">
-        <f>MAX(C118:C131)-MIN(D118:D131)</f>
+        <f t="shared" si="4"/>
         <v>18.5899</v>
       </c>
       <c r="H131" s="5">
-        <f>F131/G131*100</f>
+        <f t="shared" si="5"/>
         <v>29.047493531433748</v>
       </c>
     </row>
@@ -28876,15 +28879,15 @@
         <v>207.26</v>
       </c>
       <c r="F132">
-        <f>MAX(C119:C132)-E132</f>
+        <f t="shared" si="3"/>
         <v>7.4800000000000182</v>
       </c>
       <c r="G132">
-        <f>MAX(C119:C132)-MIN(D119:D132)</f>
+        <f t="shared" si="4"/>
         <v>18.490000000000009</v>
       </c>
       <c r="H132" s="5">
-        <f>F132/G132*100</f>
+        <f t="shared" si="5"/>
         <v>40.454299621417064</v>
       </c>
     </row>
@@ -28905,15 +28908,15 @@
         <v>210.33</v>
       </c>
       <c r="F133">
-        <f>MAX(C120:C133)-E133</f>
+        <f t="shared" si="3"/>
         <v>2.2399999999999807</v>
       </c>
       <c r="G133">
-        <f>MAX(C120:C133)-MIN(D120:D133)</f>
+        <f t="shared" si="4"/>
         <v>16.319999999999993</v>
       </c>
       <c r="H133" s="5">
-        <f>F133/G133*100</f>
+        <f t="shared" si="5"/>
         <v>13.725490196078319</v>
       </c>
     </row>
@@ -28934,15 +28937,15 @@
         <v>212.46</v>
       </c>
       <c r="F134">
-        <f>MAX(C121:C134)-E134</f>
+        <f t="shared" si="3"/>
         <v>1.5300000000000011</v>
       </c>
       <c r="G134">
-        <f>MAX(C121:C134)-MIN(D121:D134)</f>
+        <f t="shared" si="4"/>
         <v>17.740000000000009</v>
       </c>
       <c r="H134" s="5">
-        <f>F134/G134*100</f>
+        <f t="shared" si="5"/>
         <v>8.6245772266065401</v>
       </c>
     </row>
@@ -28963,15 +28966,15 @@
         <v>206.19</v>
       </c>
       <c r="F135">
-        <f>MAX(C122:C135)-E135</f>
+        <f t="shared" si="3"/>
         <v>7.8000000000000114</v>
       </c>
       <c r="G135">
-        <f>MAX(C122:C135)-MIN(D122:D135)</f>
+        <f t="shared" si="4"/>
         <v>17.740000000000009</v>
       </c>
       <c r="H135" s="5">
-        <f>F135/G135*100</f>
+        <f t="shared" si="5"/>
         <v>43.96843291995495</v>
       </c>
     </row>
@@ -28992,15 +28995,15 @@
         <v>210.38</v>
       </c>
       <c r="F136">
-        <f>MAX(C123:C136)-E136</f>
+        <f t="shared" si="3"/>
         <v>3.6100000000000136</v>
       </c>
       <c r="G136">
-        <f>MAX(C123:C136)-MIN(D123:D136)</f>
+        <f t="shared" si="4"/>
         <v>17.740000000000009</v>
       </c>
       <c r="H136" s="5">
-        <f>F136/G136*100</f>
+        <f t="shared" si="5"/>
         <v>20.349492671927912</v>
       </c>
     </row>
@@ -29021,15 +29024,15 @@
         <v>205.91</v>
       </c>
       <c r="F137">
-        <f>MAX(C124:C137)-E137</f>
+        <f t="shared" si="3"/>
         <v>8.0800000000000125</v>
       </c>
       <c r="G137">
-        <f>MAX(C124:C137)-MIN(D124:D137)</f>
+        <f t="shared" si="4"/>
         <v>17.740000000000009</v>
       </c>
       <c r="H137" s="5">
-        <f>F137/G137*100</f>
+        <f t="shared" si="5"/>
         <v>45.546786922209741</v>
       </c>
     </row>
@@ -29050,15 +29053,15 @@
         <v>209.83</v>
       </c>
       <c r="F138">
-        <f>MAX(C125:C138)-E138</f>
+        <f t="shared" si="3"/>
         <v>4.1599999999999966</v>
       </c>
       <c r="G138">
-        <f>MAX(C125:C138)-MIN(D125:D138)</f>
+        <f t="shared" si="4"/>
         <v>17.740000000000009</v>
       </c>
       <c r="H138" s="5">
-        <f>F138/G138*100</f>
+        <f t="shared" si="5"/>
         <v>23.449830890642584</v>
       </c>
     </row>
@@ -29079,15 +29082,15 @@
         <v>210.58</v>
       </c>
       <c r="F139">
-        <f>MAX(C126:C139)-E139</f>
+        <f t="shared" si="3"/>
         <v>3.4099999999999966</v>
       </c>
       <c r="G139">
-        <f>MAX(C126:C139)-MIN(D126:D139)</f>
+        <f t="shared" si="4"/>
         <v>17.610000000000014</v>
       </c>
       <c r="H139" s="5">
-        <f>F139/G139*100</f>
+        <f t="shared" si="5"/>
         <v>19.36399772856328</v>
       </c>
     </row>
@@ -29108,15 +29111,15 @@
         <v>215.81</v>
       </c>
       <c r="F140">
-        <f>MAX(C127:C140)-E140</f>
+        <f t="shared" si="3"/>
         <v>5.0000000000011369E-2</v>
       </c>
       <c r="G140">
-        <f>MAX(C127:C140)-MIN(D127:D140)</f>
+        <f t="shared" si="4"/>
         <v>16.660000000000025</v>
       </c>
       <c r="H140" s="5">
-        <f>F140/G140*100</f>
+        <f t="shared" si="5"/>
         <v>0.3001200480192755</v>
       </c>
     </row>
@@ -29137,15 +29140,15 @@
         <v>221.4</v>
       </c>
       <c r="F141">
-        <f>MAX(C128:C141)-E141</f>
+        <f t="shared" si="3"/>
         <v>2.460000000000008</v>
       </c>
       <c r="G141">
-        <f>MAX(C128:C141)-MIN(D128:D141)</f>
+        <f t="shared" si="4"/>
         <v>24.660000000000025</v>
       </c>
       <c r="H141" s="5">
-        <f>F141/G141*100</f>
+        <f t="shared" si="5"/>
         <v>9.975669099756713</v>
       </c>
     </row>
@@ -29166,15 +29169,15 @@
         <v>222.86</v>
       </c>
       <c r="F142">
-        <f>MAX(C129:C142)-E142</f>
+        <f t="shared" si="3"/>
         <v>2.3499999999999943</v>
       </c>
       <c r="G142">
-        <f>MAX(C129:C142)-MIN(D129:D142)</f>
+        <f t="shared" si="4"/>
         <v>26.010000000000019</v>
       </c>
       <c r="H142" s="5">
-        <f>F142/G142*100</f>
+        <f t="shared" si="5"/>
         <v>9.034986543637034</v>
       </c>
     </row>
@@ -29195,15 +29198,15 @@
         <v>220.86</v>
       </c>
       <c r="F143">
-        <f>MAX(C130:C143)-E143</f>
+        <f t="shared" ref="F143:F206" si="6">MAX(C130:C143)-E143</f>
         <v>4.3499999999999943</v>
       </c>
       <c r="G143">
-        <f>MAX(C130:C143)-MIN(D130:D143)</f>
+        <f t="shared" ref="G143:G206" si="7">MAX(C130:C143)-MIN(D130:D143)</f>
         <v>22.670000000000016</v>
       </c>
       <c r="H143" s="5">
-        <f>F143/G143*100</f>
+        <f t="shared" ref="H143:H206" si="8">F143/G143*100</f>
         <v>19.188354653727355</v>
       </c>
     </row>
@@ -29224,15 +29227,15 @@
         <v>219.66</v>
       </c>
       <c r="F144">
-        <f>MAX(C131:C144)-E144</f>
+        <f t="shared" si="6"/>
         <v>5.5500000000000114</v>
       </c>
       <c r="G144">
-        <f>MAX(C131:C144)-MIN(D131:D144)</f>
+        <f t="shared" si="7"/>
         <v>20.390000000000015</v>
       </c>
       <c r="H144" s="5">
-        <f>F144/G144*100</f>
+        <f t="shared" si="8"/>
         <v>27.219225110348244</v>
       </c>
     </row>
@@ -29253,15 +29256,15 @@
         <v>219.66</v>
       </c>
       <c r="F145">
-        <f>MAX(C132:C145)-E145</f>
+        <f t="shared" si="6"/>
         <v>5.5500000000000114</v>
       </c>
       <c r="G145">
-        <f>MAX(C132:C145)-MIN(D132:D145)</f>
+        <f t="shared" si="7"/>
         <v>20.390000000000015</v>
       </c>
       <c r="H145" s="5">
-        <f>F145/G145*100</f>
+        <f t="shared" si="8"/>
         <v>27.219225110348244</v>
       </c>
     </row>
@@ -29282,15 +29285,15 @@
         <v>214.22</v>
       </c>
       <c r="F146">
-        <f>MAX(C133:C146)-E146</f>
+        <f t="shared" si="6"/>
         <v>10.990000000000009</v>
       </c>
       <c r="G146">
-        <f>MAX(C133:C146)-MIN(D133:D146)</f>
+        <f t="shared" si="7"/>
         <v>20.390000000000015</v>
       </c>
       <c r="H146" s="5">
-        <f>F146/G146*100</f>
+        <f t="shared" si="8"/>
         <v>53.898970083374209</v>
       </c>
     </row>
@@ -29311,15 +29314,15 @@
         <v>214.65</v>
       </c>
       <c r="F147">
-        <f>MAX(C134:C147)-E147</f>
+        <f t="shared" si="6"/>
         <v>10.560000000000002</v>
       </c>
       <c r="G147">
-        <f>MAX(C134:C147)-MIN(D134:D147)</f>
+        <f t="shared" si="7"/>
         <v>20.390000000000015</v>
       </c>
       <c r="H147" s="5">
-        <f>F147/G147*100</f>
+        <f t="shared" si="8"/>
         <v>51.790093182932786</v>
       </c>
     </row>
@@ -29340,15 +29343,15 @@
         <v>214.8</v>
       </c>
       <c r="F148">
-        <f>MAX(C135:C148)-E148</f>
+        <f t="shared" si="6"/>
         <v>10.409999999999997</v>
       </c>
       <c r="G148">
-        <f>MAX(C135:C148)-MIN(D135:D148)</f>
+        <f t="shared" si="7"/>
         <v>20.390000000000015</v>
       </c>
       <c r="H148" s="5">
-        <f>F148/G148*100</f>
+        <f t="shared" si="8"/>
         <v>51.054438450220644</v>
       </c>
     </row>
@@ -29369,15 +29372,15 @@
         <v>214.89</v>
       </c>
       <c r="F149">
-        <f>MAX(C136:C149)-E149</f>
+        <f t="shared" si="6"/>
         <v>10.320000000000022</v>
       </c>
       <c r="G149">
-        <f>MAX(C136:C149)-MIN(D136:D149)</f>
+        <f t="shared" si="7"/>
         <v>20.390000000000015</v>
       </c>
       <c r="H149" s="5">
-        <f>F149/G149*100</f>
+        <f t="shared" si="8"/>
         <v>50.613045610593502</v>
       </c>
     </row>
@@ -29398,15 +29401,15 @@
         <v>216.23</v>
       </c>
       <c r="F150">
-        <f>MAX(C137:C150)-E150</f>
+        <f t="shared" si="6"/>
         <v>8.9800000000000182</v>
       </c>
       <c r="G150">
-        <f>MAX(C137:C150)-MIN(D137:D150)</f>
+        <f t="shared" si="7"/>
         <v>20.390000000000015</v>
       </c>
       <c r="H150" s="5">
-        <f>F150/G150*100</f>
+        <f t="shared" si="8"/>
         <v>44.041196665031933</v>
       </c>
     </row>
@@ -29427,15 +29430,15 @@
         <v>210.08</v>
       </c>
       <c r="F151">
-        <f>MAX(C138:C151)-E151</f>
+        <f t="shared" si="6"/>
         <v>15.129999999999995</v>
       </c>
       <c r="G151">
-        <f>MAX(C138:C151)-MIN(D138:D151)</f>
+        <f t="shared" si="7"/>
         <v>18.490000000000009</v>
       </c>
       <c r="H151" s="5">
-        <f>F151/G151*100</f>
+        <f t="shared" si="8"/>
         <v>81.828015143320656</v>
       </c>
     </row>
@@ -29456,15 +29459,15 @@
         <v>213.25</v>
       </c>
       <c r="F152">
-        <f>MAX(C139:C152)-E152</f>
+        <f t="shared" si="6"/>
         <v>11.960000000000008</v>
       </c>
       <c r="G152">
-        <f>MAX(C139:C152)-MIN(D139:D152)</f>
+        <f t="shared" si="7"/>
         <v>17.110000000000014</v>
       </c>
       <c r="H152" s="5">
-        <f>F152/G152*100</f>
+        <f t="shared" si="8"/>
         <v>69.900642898889529</v>
       </c>
     </row>
@@ -29485,15 +29488,15 @@
         <v>202.68</v>
       </c>
       <c r="F153">
-        <f>MAX(C140:C153)-E153</f>
+        <f t="shared" si="6"/>
         <v>22.53</v>
       </c>
       <c r="G153">
-        <f>MAX(C140:C153)-MIN(D140:D153)</f>
+        <f t="shared" si="7"/>
         <v>23.110000000000014</v>
       </c>
       <c r="H153" s="5">
-        <f>F153/G153*100</f>
+        <f t="shared" si="8"/>
         <v>97.490263954997786</v>
       </c>
     </row>
@@ -29514,15 +29517,15 @@
         <v>204.72</v>
       </c>
       <c r="F154">
-        <f>MAX(C141:C154)-E154</f>
+        <f t="shared" si="6"/>
         <v>20.490000000000009</v>
       </c>
       <c r="G154">
-        <f>MAX(C141:C154)-MIN(D141:D154)</f>
+        <f t="shared" si="7"/>
         <v>23.110000000000014</v>
       </c>
       <c r="H154" s="5">
-        <f>F154/G154*100</f>
+        <f t="shared" si="8"/>
         <v>88.662916486369525</v>
       </c>
     </row>
@@ -29543,15 +29546,15 @@
         <v>202.47</v>
       </c>
       <c r="F155">
-        <f>MAX(C142:C155)-E155</f>
+        <f t="shared" si="6"/>
         <v>22.740000000000009</v>
       </c>
       <c r="G155">
-        <f>MAX(C142:C155)-MIN(D142:D155)</f>
+        <f t="shared" si="7"/>
         <v>25.590000000000003</v>
       </c>
       <c r="H155" s="5">
-        <f>F155/G155*100</f>
+        <f t="shared" si="8"/>
         <v>88.862837045721008</v>
       </c>
     </row>
@@ -29572,15 +29575,15 @@
         <v>202.33</v>
       </c>
       <c r="F156">
-        <f>MAX(C143:C156)-E156</f>
+        <f t="shared" si="6"/>
         <v>21.889999999999986</v>
       </c>
       <c r="G156">
-        <f>MAX(C143:C156)-MIN(D143:D156)</f>
+        <f t="shared" si="7"/>
         <v>24.599999999999994</v>
       </c>
       <c r="H156" s="5">
-        <f>F156/G156*100</f>
+        <f t="shared" si="8"/>
         <v>88.983739837398332</v>
       </c>
     </row>
@@ -29601,15 +29604,15 @@
         <v>206.43</v>
       </c>
       <c r="F157">
-        <f>MAX(C144:C157)-E157</f>
+        <f t="shared" si="6"/>
         <v>15.870000000000005</v>
       </c>
       <c r="G157">
-        <f>MAX(C144:C157)-MIN(D144:D157)</f>
+        <f t="shared" si="7"/>
         <v>22.680000000000007</v>
       </c>
       <c r="H157" s="5">
-        <f>F157/G157*100</f>
+        <f t="shared" si="8"/>
         <v>69.973544973544975</v>
       </c>
     </row>
@@ -29630,15 +29633,15 @@
         <v>216.39</v>
       </c>
       <c r="F158">
-        <f>MAX(C145:C158)-E158</f>
+        <f t="shared" si="6"/>
         <v>5.910000000000025</v>
       </c>
       <c r="G158">
-        <f>MAX(C145:C158)-MIN(D145:D158)</f>
+        <f t="shared" si="7"/>
         <v>22.680000000000007</v>
       </c>
       <c r="H158" s="5">
-        <f>F158/G158*100</f>
+        <f t="shared" si="8"/>
         <v>26.058201058201156</v>
       </c>
     </row>
@@ -29659,15 +29662,15 @@
         <v>223.29</v>
       </c>
       <c r="F159">
-        <f>MAX(C146:C159)-E159</f>
+        <f t="shared" si="6"/>
         <v>0.83000000000001251</v>
       </c>
       <c r="G159">
-        <f>MAX(C146:C159)-MIN(D146:D159)</f>
+        <f t="shared" si="7"/>
         <v>24.5</v>
       </c>
       <c r="H159" s="5">
-        <f>F159/G159*100</f>
+        <f t="shared" si="8"/>
         <v>3.3877551020408672</v>
       </c>
     </row>
@@ -29688,15 +29691,15 @@
         <v>223.72</v>
       </c>
       <c r="F160">
-        <f>MAX(C147:C160)-E160</f>
+        <f t="shared" si="6"/>
         <v>0.64000000000001478</v>
       </c>
       <c r="G160">
-        <f>MAX(C147:C160)-MIN(D147:D160)</f>
+        <f t="shared" si="7"/>
         <v>24.740000000000009</v>
       </c>
       <c r="H160" s="5">
-        <f>F160/G160*100</f>
+        <f t="shared" si="8"/>
         <v>2.5869037995150146</v>
       </c>
     </row>
@@ -29717,15 +29720,15 @@
         <v>218.39</v>
       </c>
       <c r="F161">
-        <f>MAX(C148:C161)-E161</f>
+        <f t="shared" si="6"/>
         <v>9.7300000000000182</v>
       </c>
       <c r="G161">
-        <f>MAX(C148:C161)-MIN(D148:D161)</f>
+        <f t="shared" si="7"/>
         <v>28.5</v>
       </c>
       <c r="H161" s="5">
-        <f>F161/G161*100</f>
+        <f t="shared" si="8"/>
         <v>34.14035087719305</v>
       </c>
     </row>
@@ -29746,15 +29749,15 @@
         <v>211.01</v>
       </c>
       <c r="F162">
-        <f>MAX(C149:C162)-E162</f>
+        <f t="shared" si="6"/>
         <v>17.110000000000014</v>
       </c>
       <c r="G162">
-        <f>MAX(C149:C162)-MIN(D149:D162)</f>
+        <f t="shared" si="7"/>
         <v>28.5</v>
       </c>
       <c r="H162" s="5">
-        <f>F162/G162*100</f>
+        <f t="shared" si="8"/>
         <v>60.035087719298296</v>
       </c>
     </row>
@@ -29775,15 +29778,15 @@
         <v>216.55</v>
       </c>
       <c r="F163">
-        <f>MAX(C150:C163)-E163</f>
+        <f t="shared" si="6"/>
         <v>11.569999999999993</v>
       </c>
       <c r="G163">
-        <f>MAX(C150:C163)-MIN(D150:D163)</f>
+        <f t="shared" si="7"/>
         <v>28.5</v>
       </c>
       <c r="H163" s="5">
-        <f>F163/G163*100</f>
+        <f t="shared" si="8"/>
         <v>40.59649122807015</v>
       </c>
     </row>
@@ -29804,15 +29807,15 @@
         <v>215.44</v>
       </c>
       <c r="F164">
-        <f>MAX(C151:C164)-E164</f>
+        <f t="shared" si="6"/>
         <v>12.680000000000007</v>
       </c>
       <c r="G164">
-        <f>MAX(C151:C164)-MIN(D151:D164)</f>
+        <f t="shared" si="7"/>
         <v>28.5</v>
       </c>
       <c r="H164" s="5">
-        <f>F164/G164*100</f>
+        <f t="shared" si="8"/>
         <v>44.491228070175467</v>
       </c>
     </row>
@@ -29833,15 +29836,15 @@
         <v>216.51</v>
       </c>
       <c r="F165">
-        <f>MAX(C152:C165)-E165</f>
+        <f t="shared" si="6"/>
         <v>11.610000000000014</v>
       </c>
       <c r="G165">
-        <f>MAX(C152:C165)-MIN(D152:D165)</f>
+        <f t="shared" si="7"/>
         <v>28.5</v>
       </c>
       <c r="H165" s="5">
-        <f>F165/G165*100</f>
+        <f t="shared" si="8"/>
         <v>40.736842105263207</v>
       </c>
     </row>
@@ -29862,15 +29865,15 @@
         <v>217.23</v>
       </c>
       <c r="F166">
-        <f>MAX(C153:C166)-E166</f>
+        <f t="shared" si="6"/>
         <v>10.890000000000015</v>
       </c>
       <c r="G166">
-        <f>MAX(C153:C166)-MIN(D153:D166)</f>
+        <f t="shared" si="7"/>
         <v>28.5</v>
       </c>
       <c r="H166" s="5">
-        <f>F166/G166*100</f>
+        <f t="shared" si="8"/>
         <v>38.210526315789529</v>
       </c>
     </row>
@@ -29891,15 +29894,15 @@
         <v>214.46</v>
       </c>
       <c r="F167">
-        <f>MAX(C154:C167)-E167</f>
+        <f t="shared" si="6"/>
         <v>13.659999999999997</v>
       </c>
       <c r="G167">
-        <f>MAX(C154:C167)-MIN(D154:D167)</f>
+        <f t="shared" si="7"/>
         <v>28.5</v>
       </c>
       <c r="H167" s="5">
-        <f>F167/G167*100</f>
+        <f t="shared" si="8"/>
         <v>47.929824561403493</v>
       </c>
     </row>
@@ -29920,15 +29923,15 @@
         <v>211.08</v>
       </c>
       <c r="F168">
-        <f>MAX(C155:C168)-E168</f>
+        <f t="shared" si="6"/>
         <v>17.039999999999992</v>
       </c>
       <c r="G168">
-        <f>MAX(C155:C168)-MIN(D155:D168)</f>
+        <f t="shared" si="7"/>
         <v>28.5</v>
       </c>
       <c r="H168" s="5">
-        <f>F168/G168*100</f>
+        <f t="shared" si="8"/>
         <v>59.789473684210506</v>
       </c>
     </row>
@@ -29949,15 +29952,15 @@
         <v>212.42</v>
       </c>
       <c r="F169">
-        <f>MAX(C156:C169)-E169</f>
+        <f t="shared" si="6"/>
         <v>15.700000000000017</v>
       </c>
       <c r="G169">
-        <f>MAX(C156:C169)-MIN(D156:D169)</f>
+        <f t="shared" si="7"/>
         <v>28</v>
       </c>
       <c r="H169" s="5">
-        <f>F169/G169*100</f>
+        <f t="shared" si="8"/>
         <v>56.071428571428626</v>
       </c>
     </row>
@@ -29978,15 +29981,15 @@
         <v>210.39</v>
       </c>
       <c r="F170">
-        <f>MAX(C157:C170)-E170</f>
+        <f t="shared" si="6"/>
         <v>17.730000000000018</v>
       </c>
       <c r="G170">
-        <f>MAX(C157:C170)-MIN(D157:D170)</f>
+        <f t="shared" si="7"/>
         <v>25</v>
       </c>
       <c r="H170" s="5">
-        <f>F170/G170*100</f>
+        <f t="shared" si="8"/>
         <v>70.920000000000073</v>
       </c>
     </row>
@@ -30007,15 +30010,15 @@
         <v>210.11</v>
       </c>
       <c r="F171">
-        <f>MAX(C158:C171)-E171</f>
+        <f t="shared" si="6"/>
         <v>18.009999999999991</v>
       </c>
       <c r="G171">
-        <f>MAX(C158:C171)-MIN(D158:D171)</f>
+        <f t="shared" si="7"/>
         <v>19.960000000000008</v>
       </c>
       <c r="H171" s="5">
-        <f>F171/G171*100</f>
+        <f t="shared" si="8"/>
         <v>90.230460921843601</v>
       </c>
     </row>
@@ -30036,15 +30039,15 @@
         <v>213.86</v>
       </c>
       <c r="F172">
-        <f>MAX(C159:C172)-E172</f>
+        <f t="shared" si="6"/>
         <v>14.259999999999991</v>
       </c>
       <c r="G172">
-        <f>MAX(C159:C172)-MIN(D159:D172)</f>
+        <f t="shared" si="7"/>
         <v>19.960000000000008</v>
       </c>
       <c r="H172" s="5">
-        <f>F172/G172*100</f>
+        <f t="shared" si="8"/>
         <v>71.442885771543004</v>
       </c>
     </row>
@@ -30065,15 +30068,15 @@
         <v>213.87</v>
       </c>
       <c r="F173">
-        <f>MAX(C160:C173)-E173</f>
+        <f t="shared" si="6"/>
         <v>14.25</v>
       </c>
       <c r="G173">
-        <f>MAX(C160:C173)-MIN(D160:D173)</f>
+        <f t="shared" si="7"/>
         <v>19.960000000000008</v>
       </c>
       <c r="H173" s="5">
-        <f>F173/G173*100</f>
+        <f t="shared" si="8"/>
         <v>71.392785571142255</v>
       </c>
     </row>
@@ -30094,15 +30097,15 @@
         <v>215.23</v>
       </c>
       <c r="F174">
-        <f>MAX(C161:C174)-E174</f>
+        <f t="shared" si="6"/>
         <v>12.890000000000015</v>
       </c>
       <c r="G174">
-        <f>MAX(C161:C174)-MIN(D161:D174)</f>
+        <f t="shared" si="7"/>
         <v>19.960000000000008</v>
       </c>
       <c r="H174" s="5">
-        <f>F174/G174*100</f>
+        <f t="shared" si="8"/>
         <v>64.579158316633311</v>
       </c>
     </row>
@@ -30123,15 +30126,15 @@
         <v>214.07</v>
       </c>
       <c r="F175">
-        <f>MAX(C162:C175)-E175</f>
+        <f t="shared" si="6"/>
         <v>5.0400000000000205</v>
       </c>
       <c r="G175">
-        <f>MAX(C162:C175)-MIN(D162:D175)</f>
+        <f t="shared" si="7"/>
         <v>10.950000000000017</v>
       </c>
       <c r="H175" s="5">
-        <f>F175/G175*100</f>
+        <f t="shared" si="8"/>
         <v>46.027397260274086</v>
       </c>
     </row>
@@ -30152,15 +30155,15 @@
         <v>216.21</v>
       </c>
       <c r="F176">
-        <f>MAX(C163:C176)-E176</f>
+        <f t="shared" si="6"/>
         <v>2.9000000000000057</v>
       </c>
       <c r="G176">
-        <f>MAX(C163:C176)-MIN(D163:D176)</f>
+        <f t="shared" si="7"/>
         <v>10.950000000000017</v>
       </c>
       <c r="H176" s="5">
-        <f>F176/G176*100</f>
+        <f t="shared" si="8"/>
         <v>26.484018264840191</v>
       </c>
     </row>
@@ -30181,15 +30184,15 @@
         <v>215.37</v>
       </c>
       <c r="F177">
-        <f>MAX(C164:C177)-E177</f>
+        <f t="shared" si="6"/>
         <v>3.7400000000000091</v>
       </c>
       <c r="G177">
-        <f>MAX(C164:C177)-MIN(D164:D177)</f>
+        <f t="shared" si="7"/>
         <v>10.950000000000017</v>
       </c>
       <c r="H177" s="5">
-        <f>F177/G177*100</f>
+        <f t="shared" si="8"/>
         <v>34.15525114155254</v>
       </c>
     </row>
@@ -30210,15 +30213,15 @@
         <v>214.24</v>
       </c>
       <c r="F178">
-        <f>MAX(C165:C178)-E178</f>
+        <f t="shared" si="6"/>
         <v>3.5</v>
       </c>
       <c r="G178">
-        <f>MAX(C165:C178)-MIN(D165:D178)</f>
+        <f t="shared" si="7"/>
         <v>9.5800000000000125</v>
       </c>
       <c r="H178" s="5">
-        <f>F178/G178*100</f>
+        <f t="shared" si="8"/>
         <v>36.534446764091811</v>
       </c>
     </row>
@@ -30239,15 +30242,15 @@
         <v>214.36</v>
       </c>
       <c r="F179">
-        <f>MAX(C166:C179)-E179</f>
+        <f t="shared" si="6"/>
         <v>3.3799999999999955</v>
       </c>
       <c r="G179">
-        <f>MAX(C166:C179)-MIN(D166:D179)</f>
+        <f t="shared" si="7"/>
         <v>9.5800000000000125</v>
       </c>
       <c r="H179" s="5">
-        <f>F179/G179*100</f>
+        <f t="shared" si="8"/>
         <v>35.281837160751472</v>
       </c>
     </row>
@@ -30268,15 +30271,15 @@
         <v>214.29</v>
       </c>
       <c r="F180">
-        <f>MAX(C167:C180)-E180</f>
+        <f t="shared" si="6"/>
         <v>3.3900000000000148</v>
       </c>
       <c r="G180">
-        <f>MAX(C167:C180)-MIN(D167:D180)</f>
+        <f t="shared" si="7"/>
         <v>9.5200000000000102</v>
       </c>
       <c r="H180" s="5">
-        <f>F180/G180*100</f>
+        <f t="shared" si="8"/>
         <v>35.609243697479108</v>
       </c>
     </row>
@@ -30297,15 +30300,15 @@
         <v>216.01</v>
       </c>
       <c r="F181">
-        <f>MAX(C168:C181)-E181</f>
+        <f t="shared" si="6"/>
         <v>1.3100000000000023</v>
       </c>
       <c r="G181">
-        <f>MAX(C168:C181)-MIN(D168:D181)</f>
+        <f t="shared" si="7"/>
         <v>9.1599999999999966</v>
       </c>
       <c r="H181" s="5">
-        <f>F181/G181*100</f>
+        <f t="shared" si="8"/>
         <v>14.301310043668153</v>
       </c>
     </row>
@@ -30326,15 +30329,15 @@
         <v>211.8</v>
       </c>
       <c r="F182">
-        <f>MAX(C169:C182)-E182</f>
+        <f t="shared" si="6"/>
         <v>5.5199999999999818</v>
       </c>
       <c r="G182">
-        <f>MAX(C169:C182)-MIN(D169:D182)</f>
+        <f t="shared" si="7"/>
         <v>9.1599999999999966</v>
       </c>
       <c r="H182" s="5">
-        <f>F182/G182*100</f>
+        <f t="shared" si="8"/>
         <v>60.26200873362427</v>
       </c>
     </row>
@@ -30355,15 +30358,15 @@
         <v>210.52</v>
       </c>
       <c r="F183">
-        <f>MAX(C170:C183)-E183</f>
+        <f t="shared" si="6"/>
         <v>6.7999999999999829</v>
       </c>
       <c r="G183">
-        <f>MAX(C170:C183)-MIN(D170:D183)</f>
+        <f t="shared" si="7"/>
         <v>9.1599999999999966</v>
       </c>
       <c r="H183" s="5">
-        <f>F183/G183*100</f>
+        <f t="shared" si="8"/>
         <v>74.235807860261843</v>
       </c>
     </row>
@@ -30384,15 +30387,15 @@
         <v>213.26</v>
       </c>
       <c r="F184">
-        <f>MAX(C171:C184)-E184</f>
+        <f t="shared" si="6"/>
         <v>4.0600000000000023</v>
       </c>
       <c r="G184">
-        <f>MAX(C171:C184)-MIN(D171:D184)</f>
+        <f t="shared" si="7"/>
         <v>9.1599999999999966</v>
       </c>
       <c r="H184" s="5">
-        <f>F184/G184*100</f>
+        <f t="shared" si="8"/>
         <v>44.323144104803532</v>
       </c>
     </row>
@@ -30413,15 +30416,15 @@
         <v>214.2</v>
       </c>
       <c r="F185">
-        <f>MAX(C172:C185)-E185</f>
+        <f t="shared" si="6"/>
         <v>3.1200000000000045</v>
       </c>
       <c r="G185">
-        <f>MAX(C172:C185)-MIN(D172:D185)</f>
+        <f t="shared" si="7"/>
         <v>8.4599999999999795</v>
       </c>
       <c r="H185" s="5">
-        <f>F185/G185*100</f>
+        <f t="shared" si="8"/>
         <v>36.879432624113619</v>
       </c>
     </row>
@@ -30442,15 +30445,15 @@
         <v>214.13</v>
       </c>
       <c r="F186">
-        <f>MAX(C173:C186)-E186</f>
+        <f t="shared" si="6"/>
         <v>3.1899999999999977</v>
       </c>
       <c r="G186">
-        <f>MAX(C173:C186)-MIN(D173:D186)</f>
+        <f t="shared" si="7"/>
         <v>8.2099999999999795</v>
       </c>
       <c r="H186" s="5">
-        <f>F186/G186*100</f>
+        <f t="shared" si="8"/>
         <v>38.85505481120591</v>
       </c>
     </row>
@@ -30471,15 +30474,15 @@
         <v>219.28</v>
       </c>
       <c r="F187">
-        <f>MAX(C174:C187)-E187</f>
+        <f t="shared" si="6"/>
         <v>0.83000000000001251</v>
       </c>
       <c r="G187">
-        <f>MAX(C174:C187)-MIN(D174:D187)</f>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
       <c r="H187" s="5">
-        <f>F187/G187*100</f>
+        <f t="shared" si="8"/>
         <v>7.5454545454546595</v>
       </c>
     </row>
@@ -30500,15 +30503,15 @@
         <v>219.42</v>
       </c>
       <c r="F188">
-        <f>MAX(C175:C188)-E188</f>
+        <f t="shared" si="6"/>
         <v>1.4699999999999989</v>
       </c>
       <c r="G188">
-        <f>MAX(C175:C188)-MIN(D175:D188)</f>
+        <f t="shared" si="7"/>
         <v>11.779999999999973</v>
       </c>
       <c r="H188" s="5">
-        <f>F188/G188*100</f>
+        <f t="shared" si="8"/>
         <v>12.478777589134145</v>
       </c>
     </row>
@@ -30529,15 +30532,15 @@
         <v>218.59</v>
       </c>
       <c r="F189">
-        <f>MAX(C176:C189)-E189</f>
+        <f t="shared" si="6"/>
         <v>2.2999999999999829</v>
       </c>
       <c r="G189">
-        <f>MAX(C176:C189)-MIN(D176:D189)</f>
+        <f t="shared" si="7"/>
         <v>11.779999999999973</v>
       </c>
       <c r="H189" s="5">
-        <f>F189/G189*100</f>
+        <f t="shared" si="8"/>
         <v>19.524617996604317</v>
       </c>
     </row>
@@ -30558,15 +30561,15 @@
         <v>222.59</v>
       </c>
       <c r="F190">
-        <f>MAX(C177:C190)-E190</f>
+        <f t="shared" si="6"/>
         <v>1.4099999999999966</v>
       </c>
       <c r="G190">
-        <f>MAX(C177:C190)-MIN(D177:D190)</f>
+        <f t="shared" si="7"/>
         <v>14.889999999999986</v>
       </c>
       <c r="H190" s="5">
-        <f>F190/G190*100</f>
+        <f t="shared" si="8"/>
         <v>9.4694425789120071</v>
       </c>
     </row>
@@ -30587,15 +30590,15 @@
         <v>223.94</v>
       </c>
       <c r="F191">
-        <f>MAX(C178:C191)-E191</f>
+        <f t="shared" si="6"/>
         <v>1.6899999999999977</v>
       </c>
       <c r="G191">
-        <f>MAX(C178:C191)-MIN(D178:D191)</f>
+        <f t="shared" si="7"/>
         <v>16.519999999999982</v>
       </c>
       <c r="H191" s="5">
-        <f>F191/G191*100</f>
+        <f t="shared" si="8"/>
         <v>10.230024213075058</v>
       </c>
     </row>
@@ -30616,15 +30619,15 @@
         <v>221.02</v>
       </c>
       <c r="F192">
-        <f>MAX(C179:C192)-E192</f>
+        <f t="shared" si="6"/>
         <v>4.6099999999999852</v>
       </c>
       <c r="G192">
-        <f>MAX(C179:C192)-MIN(D179:D192)</f>
+        <f t="shared" si="7"/>
         <v>16.519999999999982</v>
       </c>
       <c r="H192" s="5">
-        <f>F192/G192*100</f>
+        <f t="shared" si="8"/>
         <v>27.905569007263864</v>
       </c>
     </row>
@@ -30645,15 +30648,15 @@
         <v>222.75</v>
       </c>
       <c r="F193">
-        <f>MAX(C180:C193)-E193</f>
+        <f t="shared" si="6"/>
         <v>2.8799999999999955</v>
       </c>
       <c r="G193">
-        <f>MAX(C180:C193)-MIN(D180:D193)</f>
+        <f t="shared" si="7"/>
         <v>16.519999999999982</v>
       </c>
       <c r="H193" s="5">
-        <f>F193/G193*100</f>
+        <f t="shared" si="8"/>
         <v>17.433414043583525</v>
       </c>
     </row>
@@ -30674,15 +30677,15 @@
         <v>224.96</v>
       </c>
       <c r="F194">
-        <f>MAX(C181:C194)-E194</f>
+        <f t="shared" si="6"/>
         <v>1.0699999999999932</v>
       </c>
       <c r="G194">
-        <f>MAX(C181:C194)-MIN(D181:D194)</f>
+        <f t="shared" si="7"/>
         <v>16.919999999999987</v>
       </c>
       <c r="H194" s="5">
-        <f>F194/G194*100</f>
+        <f t="shared" si="8"/>
         <v>6.3238770685578842</v>
       </c>
     </row>
@@ -30703,15 +30706,15 @@
         <v>224.15</v>
       </c>
       <c r="F195">
-        <f>MAX(C182:C195)-E195</f>
+        <f t="shared" si="6"/>
         <v>3.0300000000000011</v>
       </c>
       <c r="G195">
-        <f>MAX(C182:C195)-MIN(D182:D195)</f>
+        <f t="shared" si="7"/>
         <v>18.069999999999993</v>
       </c>
       <c r="H195" s="5">
-        <f>F195/G195*100</f>
+        <f t="shared" si="8"/>
         <v>16.768123962368577</v>
       </c>
     </row>
@@ -30732,15 +30735,15 @@
         <v>221.68</v>
       </c>
       <c r="F196">
-        <f>MAX(C183:C196)-E196</f>
+        <f t="shared" si="6"/>
         <v>5.5</v>
       </c>
       <c r="G196">
-        <f>MAX(C183:C196)-MIN(D183:D196)</f>
+        <f t="shared" si="7"/>
         <v>18.069999999999993</v>
       </c>
       <c r="H196" s="5">
-        <f>F196/G196*100</f>
+        <f t="shared" si="8"/>
         <v>30.43718871057002</v>
       </c>
     </row>
@@ -30761,15 +30764,15 @@
         <v>222.42</v>
       </c>
       <c r="F197">
-        <f>MAX(C184:C197)-E197</f>
+        <f t="shared" si="6"/>
         <v>4.7600000000000193</v>
       </c>
       <c r="G197">
-        <f>MAX(C184:C197)-MIN(D184:D197)</f>
+        <f t="shared" si="7"/>
         <v>18.069999999999993</v>
       </c>
       <c r="H197" s="5">
-        <f>F197/G197*100</f>
+        <f t="shared" si="8"/>
         <v>26.342003320420705</v>
       </c>
     </row>
@@ -30790,15 +30793,15 @@
         <v>217.69</v>
       </c>
       <c r="F198">
-        <f>MAX(C185:C198)-E198</f>
+        <f t="shared" si="6"/>
         <v>9.4900000000000091</v>
       </c>
       <c r="G198">
-        <f>MAX(C185:C198)-MIN(D185:D198)</f>
+        <f t="shared" si="7"/>
         <v>14.939999999999998</v>
       </c>
       <c r="H198" s="5">
-        <f>F198/G198*100</f>
+        <f t="shared" si="8"/>
         <v>63.520749665328047</v>
       </c>
     </row>
@@ -30819,15 +30822,15 @@
         <v>217.9</v>
       </c>
       <c r="F199">
-        <f>MAX(C186:C199)-E199</f>
+        <f t="shared" si="6"/>
         <v>9.2800000000000011</v>
       </c>
       <c r="G199">
-        <f>MAX(C186:C199)-MIN(D186:D199)</f>
+        <f t="shared" si="7"/>
         <v>14.939999999999998</v>
       </c>
       <c r="H199" s="5">
-        <f>F199/G199*100</f>
+        <f t="shared" si="8"/>
         <v>62.115127175368158</v>
       </c>
     </row>
@@ -30848,15 +30851,15 @@
         <v>212.25</v>
       </c>
       <c r="F200">
-        <f>MAX(C187:C200)-E200</f>
+        <f t="shared" si="6"/>
         <v>14.930000000000007</v>
       </c>
       <c r="G200">
-        <f>MAX(C187:C200)-MIN(D187:D200)</f>
+        <f t="shared" si="7"/>
         <v>15.240000000000009</v>
       </c>
       <c r="H200" s="5">
-        <f>F200/G200*100</f>
+        <f t="shared" si="8"/>
         <v>97.965879265091843</v>
       </c>
     </row>
@@ -30877,15 +30880,15 @@
         <v>218.29</v>
       </c>
       <c r="F201">
-        <f>MAX(C188:C201)-E201</f>
+        <f t="shared" si="6"/>
         <v>8.8900000000000148</v>
       </c>
       <c r="G201">
-        <f>MAX(C188:C201)-MIN(D188:D201)</f>
+        <f t="shared" si="7"/>
         <v>15.240000000000009</v>
       </c>
       <c r="H201" s="5">
-        <f>F201/G201*100</f>
+        <f t="shared" si="8"/>
         <v>58.333333333333393</v>
       </c>
     </row>
@@ -30906,15 +30909,15 @@
         <v>219.62</v>
       </c>
       <c r="F202">
-        <f>MAX(C189:C202)-E202</f>
+        <f t="shared" si="6"/>
         <v>7.5600000000000023</v>
       </c>
       <c r="G202">
-        <f>MAX(C189:C202)-MIN(D189:D202)</f>
+        <f t="shared" si="7"/>
         <v>15.240000000000009</v>
       </c>
       <c r="H202" s="5">
-        <f>F202/G202*100</f>
+        <f t="shared" si="8"/>
         <v>49.606299212598408</v>
       </c>
     </row>
@@ -30935,15 +30938,15 @@
         <v>217.49</v>
       </c>
       <c r="F203">
-        <f>MAX(C190:C203)-E203</f>
+        <f t="shared" si="6"/>
         <v>9.6899999999999977</v>
       </c>
       <c r="G203">
-        <f>MAX(C190:C203)-MIN(D190:D203)</f>
+        <f t="shared" si="7"/>
         <v>15.240000000000009</v>
       </c>
       <c r="H203" s="5">
-        <f>F203/G203*100</f>
+        <f t="shared" si="8"/>
         <v>63.582677165354276</v>
       </c>
     </row>
@@ -30964,15 +30967,15 @@
         <v>214.93</v>
       </c>
       <c r="F204">
-        <f>MAX(C191:C204)-E204</f>
+        <f t="shared" si="6"/>
         <v>12.25</v>
       </c>
       <c r="G204">
-        <f>MAX(C191:C204)-MIN(D191:D204)</f>
+        <f t="shared" si="7"/>
         <v>15.240000000000009</v>
       </c>
       <c r="H204" s="5">
-        <f>F204/G204*100</f>
+        <f t="shared" si="8"/>
         <v>80.380577427821478</v>
       </c>
     </row>
@@ -30993,15 +30996,15 @@
         <v>216.34</v>
       </c>
       <c r="F205">
-        <f>MAX(C192:C205)-E205</f>
+        <f t="shared" si="6"/>
         <v>10.840000000000003</v>
       </c>
       <c r="G205">
-        <f>MAX(C192:C205)-MIN(D192:D205)</f>
+        <f t="shared" si="7"/>
         <v>15.240000000000009</v>
       </c>
       <c r="H205" s="5">
-        <f>F205/G205*100</f>
+        <f t="shared" si="8"/>
         <v>71.128608923884499</v>
       </c>
     </row>
@@ -31022,15 +31025,15 @@
         <v>213.02</v>
       </c>
       <c r="F206">
-        <f>MAX(C193:C206)-E206</f>
+        <f t="shared" si="6"/>
         <v>14.159999999999997</v>
       </c>
       <c r="G206">
-        <f>MAX(C193:C206)-MIN(D193:D206)</f>
+        <f t="shared" si="7"/>
         <v>15.240000000000009</v>
       </c>
       <c r="H206" s="5">
-        <f>F206/G206*100</f>
+        <f t="shared" si="8"/>
         <v>92.913385826771574</v>
       </c>
     </row>
@@ -31051,15 +31054,15 @@
         <v>212.65</v>
       </c>
       <c r="F207">
-        <f>MAX(C194:C207)-E207</f>
+        <f t="shared" ref="F207:F250" si="9">MAX(C194:C207)-E207</f>
         <v>14.530000000000001</v>
       </c>
       <c r="G207">
-        <f>MAX(C194:C207)-MIN(D194:D207)</f>
+        <f t="shared" ref="G207:G250" si="10">MAX(C194:C207)-MIN(D194:D207)</f>
         <v>15.240000000000009</v>
       </c>
       <c r="H207" s="5">
-        <f>F207/G207*100</f>
+        <f t="shared" ref="H207:H250" si="11">F207/G207*100</f>
         <v>95.341207349081316</v>
       </c>
     </row>
@@ -31080,15 +31083,15 @@
         <v>216.44</v>
       </c>
       <c r="F208">
-        <f>MAX(C195:C208)-E208</f>
+        <f t="shared" si="9"/>
         <v>10.740000000000009</v>
       </c>
       <c r="G208">
-        <f>MAX(C195:C208)-MIN(D195:D208)</f>
+        <f t="shared" si="10"/>
         <v>15.240000000000009</v>
       </c>
       <c r="H208" s="5">
-        <f>F208/G208*100</f>
+        <f t="shared" si="11"/>
         <v>70.47244094488191</v>
       </c>
     </row>
@@ -31109,15 +31112,15 @@
         <v>224.34</v>
       </c>
       <c r="F209">
-        <f>MAX(C196:C209)-E209</f>
+        <f t="shared" si="9"/>
         <v>1.4499999999999886</v>
       </c>
       <c r="G209">
-        <f>MAX(C196:C209)-MIN(D196:D209)</f>
+        <f t="shared" si="10"/>
         <v>13.849999999999994</v>
       </c>
       <c r="H209" s="5">
-        <f>F209/G209*100</f>
+        <f t="shared" si="11"/>
         <v>10.469314079422306</v>
       </c>
     </row>
@@ -31138,15 +31141,15 @@
         <v>224.97</v>
       </c>
       <c r="F210">
-        <f>MAX(C197:C210)-E210</f>
+        <f t="shared" si="9"/>
         <v>1.3300000000000125</v>
       </c>
       <c r="G210">
-        <f>MAX(C197:C210)-MIN(D197:D210)</f>
+        <f t="shared" si="10"/>
         <v>14.360000000000014</v>
       </c>
       <c r="H210" s="5">
-        <f>F210/G210*100</f>
+        <f t="shared" si="11"/>
         <v>9.2618384401114984</v>
       </c>
     </row>
@@ -31167,15 +31170,15 @@
         <v>225.95</v>
       </c>
       <c r="F211">
-        <f>MAX(C198:C211)-E211</f>
+        <f t="shared" si="9"/>
         <v>4.1200000000000045</v>
       </c>
       <c r="G211">
-        <f>MAX(C198:C211)-MIN(D198:D211)</f>
+        <f t="shared" si="10"/>
         <v>18.129999999999995</v>
       </c>
       <c r="H211" s="5">
-        <f>F211/G211*100</f>
+        <f t="shared" si="11"/>
         <v>22.724765581908471</v>
       </c>
     </row>
@@ -31196,15 +31199,15 @@
         <v>229.53</v>
       </c>
       <c r="F212">
-        <f>MAX(C199:C212)-E212</f>
+        <f t="shared" si="9"/>
         <v>0.53999999999999204</v>
       </c>
       <c r="G212">
-        <f>MAX(C199:C212)-MIN(D199:D212)</f>
+        <f t="shared" si="10"/>
         <v>18.129999999999995</v>
       </c>
       <c r="H212" s="5">
-        <f>F212/G212*100</f>
+        <f t="shared" si="11"/>
         <v>2.9784886927743637</v>
       </c>
     </row>
@@ -31225,15 +31228,15 @@
         <v>232.33</v>
       </c>
       <c r="F213">
-        <f>MAX(C200:C213)-E213</f>
+        <f t="shared" si="9"/>
         <v>1.8499999999999943</v>
       </c>
       <c r="G213">
-        <f>MAX(C200:C213)-MIN(D200:D213)</f>
+        <f t="shared" si="10"/>
         <v>22.240000000000009</v>
       </c>
       <c r="H213" s="5">
-        <f>F213/G213*100</f>
+        <f t="shared" si="11"/>
         <v>8.3183453237409779</v>
       </c>
     </row>
@@ -31254,15 +31257,15 @@
         <v>232.9</v>
       </c>
       <c r="F214">
-        <f>MAX(C201:C214)-E214</f>
+        <f t="shared" si="9"/>
         <v>7.539999999999992</v>
       </c>
       <c r="G214">
-        <f>MAX(C201:C214)-MIN(D201:D214)</f>
+        <f t="shared" si="10"/>
         <v>28.409999999999997</v>
       </c>
       <c r="H214" s="5">
-        <f>F214/G214*100</f>
+        <f t="shared" si="11"/>
         <v>26.539950721576883</v>
       </c>
     </row>
@@ -31283,15 +31286,15 @@
         <v>238.93</v>
       </c>
       <c r="F215">
-        <f>MAX(C202:C215)-E215</f>
+        <f t="shared" si="9"/>
         <v>3.7099999999999795</v>
       </c>
       <c r="G215">
-        <f>MAX(C202:C215)-MIN(D202:D215)</f>
+        <f t="shared" si="10"/>
         <v>30.609999999999985</v>
       </c>
       <c r="H215" s="5">
-        <f>F215/G215*100</f>
+        <f t="shared" si="11"/>
         <v>12.120222149624245</v>
       </c>
     </row>
@@ -31312,15 +31315,15 @@
         <v>231.96</v>
       </c>
       <c r="F216">
-        <f>MAX(C203:C216)-E216</f>
+        <f t="shared" si="9"/>
         <v>10.679999999999978</v>
       </c>
       <c r="G216">
-        <f>MAX(C203:C216)-MIN(D203:D216)</f>
+        <f t="shared" si="10"/>
         <v>30.609999999999985</v>
       </c>
       <c r="H216" s="5">
-        <f>F216/G216*100</f>
+        <f t="shared" si="11"/>
         <v>34.890558640966951</v>
       </c>
     </row>
@@ -31341,15 +31344,15 @@
         <v>239.65</v>
       </c>
       <c r="F217">
-        <f>MAX(C204:C217)-E217</f>
+        <f t="shared" si="9"/>
         <v>2.9899999999999807</v>
       </c>
       <c r="G217">
-        <f>MAX(C204:C217)-MIN(D204:D217)</f>
+        <f t="shared" si="10"/>
         <v>30.609999999999985</v>
       </c>
       <c r="H217" s="5">
-        <f>F217/G217*100</f>
+        <f t="shared" si="11"/>
         <v>9.768049656974787</v>
       </c>
     </row>
@@ -31370,15 +31373,15 @@
         <v>239.51</v>
       </c>
       <c r="F218">
-        <f>MAX(C205:C218)-E218</f>
+        <f t="shared" si="9"/>
         <v>3.1299999999999955</v>
       </c>
       <c r="G218">
-        <f>MAX(C205:C218)-MIN(D205:D218)</f>
+        <f t="shared" si="10"/>
         <v>30.609999999999985</v>
       </c>
       <c r="H218" s="5">
-        <f>F218/G218*100</f>
+        <f t="shared" si="11"/>
         <v>10.225416530545564</v>
       </c>
     </row>
@@ -31399,15 +31402,15 @@
         <v>243</v>
       </c>
       <c r="F219">
-        <f>MAX(C206:C219)-E219</f>
+        <f t="shared" si="9"/>
         <v>2.0900000000000034</v>
       </c>
       <c r="G219">
-        <f>MAX(C206:C219)-MIN(D206:D219)</f>
+        <f t="shared" si="10"/>
         <v>33.06</v>
       </c>
       <c r="H219" s="5">
-        <f>F219/G219*100</f>
+        <f t="shared" si="11"/>
         <v>6.3218390804597808</v>
       </c>
     </row>
@@ -31428,15 +31431,15 @@
         <v>242.01</v>
       </c>
       <c r="F220">
-        <f>MAX(C207:C220)-E220</f>
+        <f t="shared" si="9"/>
         <v>3.0800000000000125</v>
       </c>
       <c r="G220">
-        <f>MAX(C207:C220)-MIN(D207:D220)</f>
+        <f t="shared" si="10"/>
         <v>33.06</v>
       </c>
       <c r="H220" s="5">
-        <f>F220/G220*100</f>
+        <f t="shared" si="11"/>
         <v>9.3163944343618041</v>
       </c>
     </row>
@@ -31457,15 +31460,15 @@
         <v>242.2</v>
       </c>
       <c r="F221">
-        <f>MAX(C208:C221)-E221</f>
+        <f t="shared" si="9"/>
         <v>2.8900000000000148</v>
       </c>
       <c r="G221">
-        <f>MAX(C208:C221)-MIN(D208:D221)</f>
+        <f t="shared" si="10"/>
         <v>32.460000000000008</v>
       </c>
       <c r="H221" s="5">
-        <f>F221/G221*100</f>
+        <f t="shared" si="11"/>
         <v>8.9032655576094086</v>
       </c>
     </row>
@@ -31486,15 +31489,15 @@
         <v>242.47</v>
       </c>
       <c r="F222">
-        <f>MAX(C209:C222)-E222</f>
+        <f t="shared" si="9"/>
         <v>2.6200000000000045</v>
       </c>
       <c r="G222">
-        <f>MAX(C209:C222)-MIN(D209:D222)</f>
+        <f t="shared" si="10"/>
         <v>27.799200000000013</v>
       </c>
       <c r="H222" s="5">
-        <f>F222/G222*100</f>
+        <f t="shared" si="11"/>
         <v>9.4247316469538802</v>
       </c>
     </row>
@@ -31515,15 +31518,15 @@
         <v>243.77</v>
       </c>
       <c r="F223">
-        <f>MAX(C210:C223)-E223</f>
+        <f t="shared" si="9"/>
         <v>1.3199999999999932</v>
       </c>
       <c r="G223">
-        <f>MAX(C210:C223)-MIN(D210:D223)</f>
+        <f t="shared" si="10"/>
         <v>22.670000000000016</v>
       </c>
       <c r="H223" s="5">
-        <f>F223/G223*100</f>
+        <f t="shared" si="11"/>
         <v>5.8226731363034512</v>
       </c>
     </row>
@@ -31544,15 +31547,15 @@
         <v>242.82</v>
       </c>
       <c r="F224">
-        <f>MAX(C211:C224)-E224</f>
+        <f t="shared" si="9"/>
         <v>3.0999999999999943</v>
       </c>
       <c r="G224">
-        <f>MAX(C211:C224)-MIN(D211:D224)</f>
+        <f t="shared" si="10"/>
         <v>21.699999999999989</v>
       </c>
       <c r="H224" s="5">
-        <f>F224/G224*100</f>
+        <f t="shared" si="11"/>
         <v>14.285714285714269</v>
       </c>
     </row>
@@ -31573,15 +31576,15 @@
         <v>244.49</v>
       </c>
       <c r="F225">
-        <f>MAX(C212:C225)-E225</f>
+        <f t="shared" si="9"/>
         <v>1.4299999999999784</v>
       </c>
       <c r="G225">
-        <f>MAX(C212:C225)-MIN(D212:D225)</f>
+        <f t="shared" si="10"/>
         <v>21.699999999999989</v>
       </c>
       <c r="H225" s="5">
-        <f>F225/G225*100</f>
+        <f t="shared" si="11"/>
         <v>6.5898617511519779</v>
       </c>
     </row>
@@ -31602,15 +31605,15 @@
         <v>244.99</v>
       </c>
       <c r="F226">
-        <f>MAX(C213:C226)-E226</f>
+        <f t="shared" si="9"/>
         <v>0.9299999999999784</v>
       </c>
       <c r="G226">
-        <f>MAX(C213:C226)-MIN(D213:D226)</f>
+        <f t="shared" si="10"/>
         <v>15.839999999999975</v>
       </c>
       <c r="H226" s="5">
-        <f>F226/G226*100</f>
+        <f t="shared" si="11"/>
         <v>5.8712121212119941</v>
       </c>
     </row>
@@ -31631,15 +31634,15 @@
         <v>243.7</v>
       </c>
       <c r="F227">
-        <f>MAX(C214:C227)-E227</f>
+        <f t="shared" si="9"/>
         <v>2.4300000000000068</v>
       </c>
       <c r="G227">
-        <f>MAX(C214:C227)-MIN(D214:D227)</f>
+        <f t="shared" si="10"/>
         <v>15.990000000000009</v>
       </c>
       <c r="H227" s="5">
-        <f>F227/G227*100</f>
+        <f t="shared" si="11"/>
         <v>15.196998123827427</v>
       </c>
     </row>
@@ -31660,15 +31663,15 @@
         <v>244.2</v>
       </c>
       <c r="F228">
-        <f>MAX(C215:C228)-E228</f>
+        <f t="shared" si="9"/>
         <v>1.9300000000000068</v>
       </c>
       <c r="G228">
-        <f>MAX(C215:C228)-MIN(D215:D228)</f>
+        <f t="shared" si="10"/>
         <v>14.780000000000001</v>
       </c>
       <c r="H228" s="5">
-        <f>F228/G228*100</f>
+        <f t="shared" si="11"/>
         <v>13.05818673883631</v>
       </c>
     </row>
@@ -31689,15 +31692,15 @@
         <v>243.79</v>
       </c>
       <c r="F229">
-        <f>MAX(C216:C229)-E229</f>
+        <f t="shared" si="9"/>
         <v>2.3400000000000034</v>
       </c>
       <c r="G229">
-        <f>MAX(C216:C229)-MIN(D216:D229)</f>
+        <f t="shared" si="10"/>
         <v>14.780000000000001</v>
       </c>
       <c r="H229" s="5">
-        <f>F229/G229*100</f>
+        <f t="shared" si="11"/>
         <v>15.832205683355907</v>
       </c>
     </row>
@@ -31718,15 +31721,15 @@
         <v>240.97</v>
       </c>
       <c r="F230">
-        <f>MAX(C217:C230)-E230</f>
+        <f t="shared" si="9"/>
         <v>5.1599999999999966</v>
       </c>
       <c r="G230">
-        <f>MAX(C217:C230)-MIN(D217:D230)</f>
+        <f t="shared" si="10"/>
         <v>13.699999999999989</v>
       </c>
       <c r="H230" s="5">
-        <f>F230/G230*100</f>
+        <f t="shared" si="11"/>
         <v>37.664233576642339</v>
       </c>
     </row>
@@ -31747,15 +31750,15 @@
         <v>234.51</v>
       </c>
       <c r="F231">
-        <f>MAX(C218:C231)-E231</f>
+        <f t="shared" si="9"/>
         <v>11.620000000000005</v>
       </c>
       <c r="G231">
-        <f>MAX(C218:C231)-MIN(D218:D231)</f>
+        <f t="shared" si="10"/>
         <v>13.72999999999999</v>
       </c>
       <c r="H231" s="5">
-        <f>F231/G231*100</f>
+        <f t="shared" si="11"/>
         <v>84.632192279679629</v>
       </c>
     </row>
@@ -31776,15 +31779,15 @@
         <v>233.27</v>
       </c>
       <c r="F232">
-        <f>MAX(C219:C232)-E232</f>
+        <f t="shared" si="9"/>
         <v>12.859999999999985</v>
       </c>
       <c r="G232">
-        <f>MAX(C219:C232)-MIN(D219:D232)</f>
+        <f t="shared" si="10"/>
         <v>17.400000000000006</v>
       </c>
       <c r="H232" s="5">
-        <f>F232/G232*100</f>
+        <f t="shared" si="11"/>
         <v>73.908045977011383</v>
       </c>
     </row>
@@ -31805,15 +31808,15 @@
         <v>234.55</v>
       </c>
       <c r="F233">
-        <f>MAX(C220:C233)-E233</f>
+        <f t="shared" si="9"/>
         <v>11.579999999999984</v>
       </c>
       <c r="G233">
-        <f>MAX(C220:C233)-MIN(D220:D233)</f>
+        <f t="shared" si="10"/>
         <v>17.400000000000006</v>
       </c>
       <c r="H233" s="5">
-        <f>F233/G233*100</f>
+        <f t="shared" si="11"/>
         <v>66.551724137930918</v>
       </c>
     </row>
@@ -31834,15 +31837,15 @@
         <v>228.99</v>
       </c>
       <c r="F234">
-        <f>MAX(C221:C234)-E234</f>
+        <f t="shared" si="9"/>
         <v>17.139999999999986</v>
       </c>
       <c r="G234">
-        <f>MAX(C221:C234)-MIN(D221:D234)</f>
+        <f t="shared" si="10"/>
         <v>18.25</v>
       </c>
       <c r="H234" s="5">
-        <f>F234/G234*100</f>
+        <f t="shared" si="11"/>
         <v>93.917808219178013</v>
       </c>
     </row>
@@ -31863,15 +31866,15 @@
         <v>232.38</v>
       </c>
       <c r="F235">
-        <f>MAX(C222:C235)-E235</f>
+        <f t="shared" si="9"/>
         <v>13.75</v>
       </c>
       <c r="G235">
-        <f>MAX(C222:C235)-MIN(D222:D235)</f>
+        <f t="shared" si="10"/>
         <v>18.25</v>
       </c>
       <c r="H235" s="5">
-        <f>F235/G235*100</f>
+        <f t="shared" si="11"/>
         <v>75.342465753424662</v>
       </c>
     </row>
@@ -31892,15 +31895,15 @@
         <v>236.94</v>
       </c>
       <c r="F236">
-        <f>MAX(C223:C236)-E236</f>
+        <f t="shared" si="9"/>
         <v>9.1899999999999977</v>
       </c>
       <c r="G236">
-        <f>MAX(C223:C236)-MIN(D223:D236)</f>
+        <f t="shared" si="10"/>
         <v>18.25</v>
       </c>
       <c r="H236" s="5">
-        <f>F236/G236*100</f>
+        <f t="shared" si="11"/>
         <v>50.356164383561634</v>
       </c>
     </row>
@@ -31921,15 +31924,15 @@
         <v>233.87</v>
       </c>
       <c r="F237">
-        <f>MAX(C224:C237)-E237</f>
+        <f t="shared" si="9"/>
         <v>12.259999999999991</v>
       </c>
       <c r="G237">
-        <f>MAX(C224:C237)-MIN(D224:D237)</f>
+        <f t="shared" si="10"/>
         <v>18.25</v>
       </c>
       <c r="H237" s="5">
-        <f>F237/G237*100</f>
+        <f t="shared" si="11"/>
         <v>67.178082191780774</v>
       </c>
     </row>
@@ -31950,15 +31953,15 @@
         <v>227.56</v>
       </c>
       <c r="F238">
-        <f>MAX(C225:C238)-E238</f>
+        <f t="shared" si="9"/>
         <v>18.569999999999993</v>
       </c>
       <c r="G238">
-        <f>MAX(C225:C238)-MIN(D225:D238)</f>
+        <f t="shared" si="10"/>
         <v>18.870000000000005</v>
       </c>
       <c r="H238" s="5">
-        <f>F238/G238*100</f>
+        <f t="shared" si="11"/>
         <v>98.410174880763051</v>
       </c>
     </row>
@@ -31979,15 +31982,15 @@
         <v>226.73</v>
       </c>
       <c r="F239">
-        <f>MAX(C226:C239)-E239</f>
+        <f t="shared" si="9"/>
         <v>19.400000000000006</v>
       </c>
       <c r="G239">
-        <f>MAX(C226:C239)-MIN(D226:D239)</f>
+        <f t="shared" si="10"/>
         <v>21.870000000000005</v>
       </c>
       <c r="H239" s="5">
-        <f>F239/G239*100</f>
+        <f t="shared" si="11"/>
         <v>88.705989940557856</v>
       </c>
     </row>
@@ -32008,15 +32011,15 @@
         <v>231.6</v>
       </c>
       <c r="F240">
-        <f>MAX(C227:C240)-E240</f>
+        <f t="shared" si="9"/>
         <v>14.530000000000001</v>
       </c>
       <c r="G240">
-        <f>MAX(C227:C240)-MIN(D227:D240)</f>
+        <f t="shared" si="10"/>
         <v>21.870000000000005</v>
       </c>
       <c r="H240" s="5">
-        <f>F240/G240*100</f>
+        <f t="shared" si="11"/>
         <v>66.438042981252849</v>
       </c>
     </row>
@@ -32037,15 +32040,15 @@
         <v>227.39</v>
       </c>
       <c r="F241">
-        <f>MAX(C228:C241)-E241</f>
+        <f t="shared" si="9"/>
         <v>16.920000000000016</v>
       </c>
       <c r="G241">
-        <f>MAX(C228:C241)-MIN(D228:D241)</f>
+        <f t="shared" si="10"/>
         <v>20.050000000000011</v>
       </c>
       <c r="H241" s="5">
-        <f>F241/G241*100</f>
+        <f t="shared" si="11"/>
         <v>84.389027431421482</v>
       </c>
     </row>
@@ -32066,15 +32069,15 @@
         <v>233.78</v>
       </c>
       <c r="F242">
-        <f>MAX(C229:C242)-E242</f>
+        <f t="shared" si="9"/>
         <v>10.150000000000006</v>
       </c>
       <c r="G242">
-        <f>MAX(C229:C242)-MIN(D229:D242)</f>
+        <f t="shared" si="10"/>
         <v>19.670000000000016</v>
       </c>
       <c r="H242" s="5">
-        <f>F242/G242*100</f>
+        <f t="shared" si="11"/>
         <v>51.601423487544473</v>
       </c>
     </row>
@@ -32095,15 +32098,15 @@
         <v>232.42</v>
       </c>
       <c r="F243">
-        <f>MAX(C230:C243)-E243</f>
+        <f t="shared" si="9"/>
         <v>11.440000000000026</v>
       </c>
       <c r="G243">
-        <f>MAX(C230:C243)-MIN(D230:D243)</f>
+        <f t="shared" si="10"/>
         <v>19.600000000000023</v>
       </c>
       <c r="H243" s="5">
-        <f>F243/G243*100</f>
+        <f t="shared" si="11"/>
         <v>58.367346938775576</v>
       </c>
     </row>
@@ -32124,15 +32127,15 @@
         <v>237.13</v>
       </c>
       <c r="F244">
-        <f>MAX(C231:C244)-E244</f>
+        <f t="shared" si="9"/>
         <v>2.039999999999992</v>
       </c>
       <c r="G244">
-        <f>MAX(C231:C244)-MIN(D231:D244)</f>
+        <f t="shared" si="10"/>
         <v>14.909999999999997</v>
       </c>
       <c r="H244" s="5">
-        <f>F244/G244*100</f>
+        <f t="shared" si="11"/>
         <v>13.682092555331943</v>
       </c>
     </row>
@@ -32153,15 +32156,15 @@
         <v>235.75</v>
       </c>
       <c r="F245">
-        <f>MAX(C232:C245)-E245</f>
+        <f t="shared" si="9"/>
         <v>3.4199999999999875</v>
       </c>
       <c r="G245">
-        <f>MAX(C232:C245)-MIN(D232:D245)</f>
+        <f t="shared" si="10"/>
         <v>14.909999999999997</v>
       </c>
       <c r="H245" s="5">
-        <f>F245/G245*100</f>
+        <f t="shared" si="11"/>
         <v>22.937625754527087</v>
       </c>
     </row>
@@ -32182,15 +32185,15 @@
         <v>234.81</v>
       </c>
       <c r="F246">
-        <f>MAX(C233:C246)-E246</f>
+        <f t="shared" si="9"/>
         <v>4.3599999999999852</v>
       </c>
       <c r="G246">
-        <f>MAX(C233:C246)-MIN(D233:D246)</f>
+        <f t="shared" si="10"/>
         <v>14.909999999999997</v>
       </c>
       <c r="H246" s="5">
-        <f>F246/G246*100</f>
+        <f t="shared" si="11"/>
         <v>29.242119382964361</v>
       </c>
     </row>
@@ -32211,15 +32214,15 @@
         <v>237.71</v>
       </c>
       <c r="F247">
-        <f>MAX(C234:C247)-E247</f>
+        <f t="shared" si="9"/>
         <v>2.3449999999999989</v>
       </c>
       <c r="G247">
-        <f>MAX(C234:C247)-MIN(D234:D247)</f>
+        <f t="shared" si="10"/>
         <v>15.795000000000016</v>
       </c>
       <c r="H247" s="5">
-        <f>F247/G247*100</f>
+        <f t="shared" si="11"/>
         <v>14.846470402025936</v>
       </c>
     </row>
@@ -32240,15 +32243,15 @@
         <v>237.04</v>
       </c>
       <c r="F248">
-        <f>MAX(C235:C248)-E248</f>
+        <f t="shared" si="9"/>
         <v>3.0150000000000148</v>
       </c>
       <c r="G248">
-        <f>MAX(C235:C248)-MIN(D235:D248)</f>
+        <f t="shared" si="10"/>
         <v>15.795000000000016</v>
       </c>
       <c r="H248" s="5">
-        <f>F248/G248*100</f>
+        <f t="shared" si="11"/>
         <v>19.088319088319164</v>
       </c>
     </row>
@@ -32269,15 +32272,15 @@
         <v>230.72</v>
       </c>
       <c r="F249">
-        <f>MAX(C236:C249)-E249</f>
+        <f t="shared" si="9"/>
         <v>9.335000000000008</v>
       </c>
       <c r="G249">
-        <f>MAX(C236:C249)-MIN(D236:D249)</f>
+        <f t="shared" si="10"/>
         <v>15.795000000000016</v>
       </c>
       <c r="H249" s="5">
-        <f>F249/G249*100</f>
+        <f t="shared" si="11"/>
         <v>59.100981323203541</v>
       </c>
     </row>
@@ -32298,19 +32301,20 @@
         <v>230.35</v>
       </c>
       <c r="F250">
-        <f>MAX(C237:C250)-E250</f>
+        <f t="shared" si="9"/>
         <v>9.7050000000000125</v>
       </c>
       <c r="G250">
-        <f>MAX(C237:C250)-MIN(D237:D250)</f>
+        <f t="shared" si="10"/>
         <v>15.795000000000016</v>
       </c>
       <c r="H250" s="5">
-        <f>F250/G250*100</f>
+        <f t="shared" si="11"/>
         <v>61.443494776828125</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>